<commit_message>
Add second dimension for bias features
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Code/eliminating-bias-in-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4B1F8A-00AD-AA47-9060-E96022E5697B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A825C09-F476-7C4A-9212-72FD6313DA25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="38680" yWindow="8280" windowWidth="37840" windowHeight="34860" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gender" sheetId="1" r:id="rId1"/>
+    <sheet name="Gender &amp; Race" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="row">Sheet1!$B$3</definedName>
+    <definedName name="row">Gender!$B$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="38">
   <si>
     <t>Training time</t>
   </si>
@@ -82,13 +83,73 @@
   </si>
   <si>
     <t>Bias Factor</t>
+  </si>
+  <si>
+    <t>&gt;50K</t>
+  </si>
+  <si>
+    <t>proportion</t>
+  </si>
+  <si>
+    <t>new n points</t>
+  </si>
+  <si>
+    <t>n additional points</t>
+  </si>
+  <si>
+    <t>bias factor</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Amer-Indian-Eskimo</t>
+  </si>
+  <si>
+    <t>Asian-Pac-Islander</t>
+  </si>
+  <si>
+    <t>npoints</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>n points</t>
+  </si>
+  <si>
+    <t>White-Asian-Pac-Islander</t>
+  </si>
+  <si>
+    <t>not White-Asian-Pac-Islander</t>
+  </si>
+  <si>
+    <t>&lt;=50K</t>
+  </si>
+  <si>
+    <t>Female &amp; not White-Asian-Pac-Islander</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,6 +178,39 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF101620"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF768096"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF101620"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -135,18 +229,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696E6750-176D-D440-9C29-55247F651D54}">
   <dimension ref="B2:M134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L96" sqref="L96"/>
     </sheetView>
   </sheetViews>
@@ -2708,4 +2814,793 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
+  <dimension ref="A1:O47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1641</v>
+      </c>
+      <c r="H3" s="5">
+        <v>8305</v>
+      </c>
+      <c r="I3" s="4">
+        <f>SUM(G3:H3)</f>
+        <v>9946</v>
+      </c>
+      <c r="N3">
+        <f>N4/(N4+N5)</f>
+        <v>0.88618285679186759</v>
+      </c>
+      <c r="O3">
+        <f>M6/SUM(M6:M11)</f>
+        <v>0.8542735173981143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <f>SUM(G3:H4)</f>
+        <v>30000</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1777</v>
+      </c>
+      <c r="H4" s="5">
+        <v>18277</v>
+      </c>
+      <c r="I4" s="4">
+        <f>SUM(G4:H4)</f>
+        <v>20054</v>
+      </c>
+      <c r="N4">
+        <f>M6+M8</f>
+        <v>28855</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
+        <f>SUM(G3:G4)</f>
+        <v>3418</v>
+      </c>
+      <c r="H5" s="4">
+        <f>SUM(H3:H4)</f>
+        <v>26582</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="N5">
+        <f>M7+M9+M10</f>
+        <v>3706</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="L6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="10">
+        <v>27816</v>
+      </c>
+      <c r="N6" s="8">
+        <f>M6/SUM($M$6:$M$10)</f>
+        <v>0.8542735173981143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="5">
+        <v>101</v>
+      </c>
+      <c r="H7" s="5">
+        <v>982</v>
+      </c>
+      <c r="I7" s="4">
+        <f>SUM(G7:H7)</f>
+        <v>1083</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="10">
+        <v>3124</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" ref="N7:N10" si="0">M7/SUM($M$6:$M$10)</f>
+        <v>9.5942999293633494E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="5">
+        <v>315</v>
+      </c>
+      <c r="H8" s="5">
+        <v>5826</v>
+      </c>
+      <c r="I8" s="4">
+        <f>SUM(G8:H8)</f>
+        <v>6141</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="10">
+        <v>1039</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1909339393753261E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4">
+        <f>SUM(G7:G8)</f>
+        <v>416</v>
+      </c>
+      <c r="H9" s="4">
+        <f>SUM(H7:H8)</f>
+        <v>6808</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="L9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="10">
+        <v>311</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="0"/>
+        <v>9.551303706888609E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="L10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="10">
+        <v>271</v>
+      </c>
+      <c r="N10" s="8">
+        <f t="shared" si="0"/>
+        <v>8.3228402076103315E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <f>G7/G3</f>
+        <v>6.1547836684948204E-2</v>
+      </c>
+      <c r="C11" s="4">
+        <f>H7/H3</f>
+        <v>0.11824202287778447</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="5">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.1182</v>
+      </c>
+      <c r="I11" s="4">
+        <f>I7/I3</f>
+        <v>0.10888799517393927</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <f>G8/G4</f>
+        <v>0.17726505346088914</v>
+      </c>
+      <c r="C12" s="4">
+        <f>H8/H4</f>
+        <v>0.31876128467472781</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.17730000000000001</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I12" s="4">
+        <f>I8/I4</f>
+        <v>0.30622319736710879</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4">
+        <f>G9/G5</f>
+        <v>0.12170860152135751</v>
+      </c>
+      <c r="H13" s="4">
+        <f>H9/H5</f>
+        <v>0.25611315928071626</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4">
+        <f>$H$12/G11</f>
+        <v>5.1837398373983739</v>
+      </c>
+      <c r="H15" s="4">
+        <f>$H$12/H11</f>
+        <v>2.6971235194585446</v>
+      </c>
+      <c r="I15" s="4">
+        <f>I12/I11</f>
+        <v>2.8122769353769752</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4">
+        <f>$H$12/G12</f>
+        <v>1.7980823463056963</v>
+      </c>
+      <c r="H16" s="4">
+        <f>$H$12/H12</f>
+        <v>1</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>619.58789999999999</v>
+      </c>
+      <c r="C17">
+        <v>2444.5385999999999</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
+        <f>H13/G13</f>
+        <v>2.1043143712055006</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>369.09059999999999</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="4">
+        <v>422.55772357723578</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1666.5752961082908</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4">
+        <f>($H$12*G3 - G7)/(1 - $H$12)</f>
+        <v>619.71638285378742</v>
+      </c>
+      <c r="H19" s="4">
+        <f>($H$12*H3-H7)/(1-$H$12)</f>
+        <v>2445.1467997651198</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="4">
+        <v>251.39593908629433</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4">
+        <f>($H$12*G4-G8)/(1-$H$12)</f>
+        <v>369.21256605989419</v>
+      </c>
+      <c r="H20" s="4">
+        <f>($H$12*H4-H8)/(1-$H$12)</f>
+        <v>1.0387551379913817</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4">
+        <f>G3+G19</f>
+        <v>2260.7163828537873</v>
+      </c>
+      <c r="H23" s="4">
+        <f>H3+H19</f>
+        <v>10750.14679976512</v>
+      </c>
+      <c r="I23" s="4">
+        <f>SUM(G23:H23)</f>
+        <v>13010.863182618907</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4">
+        <f>G4+G20</f>
+        <v>2146.212566059894</v>
+      </c>
+      <c r="H24" s="4">
+        <f>H4+H20</f>
+        <v>18278.03875513799</v>
+      </c>
+      <c r="I24" s="4">
+        <f>SUM(G24:H24)</f>
+        <v>20424.251321197884</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4">
+        <f>SUM(G23:G24)</f>
+        <v>4406.9289489136809</v>
+      </c>
+      <c r="H25" s="4">
+        <f>SUM(H23:H24)</f>
+        <v>29028.18555490311</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="4">
+        <f>G15*G7</f>
+        <v>523.55772357723572</v>
+      </c>
+      <c r="C27" s="4">
+        <f>H15*H7</f>
+        <v>2648.5752961082908</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4">
+        <f>G19+G7</f>
+        <v>720.71638285378742</v>
+      </c>
+      <c r="H27" s="4">
+        <f>H19+H7</f>
+        <v>3427.1467997651198</v>
+      </c>
+      <c r="I27" s="4">
+        <f>SUM(G27:H27)</f>
+        <v>4147.8631826189076</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="4">
+        <f>G16*G8</f>
+        <v>566.39593908629433</v>
+      </c>
+      <c r="C28" s="4">
+        <f>H16*H8</f>
+        <v>5826</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4">
+        <f>G20+G8</f>
+        <v>684.21256605989424</v>
+      </c>
+      <c r="H28" s="4">
+        <f>H20+H8</f>
+        <v>5827.0387551379918</v>
+      </c>
+      <c r="I28" s="4">
+        <f>SUM(G28:H28)</f>
+        <v>6511.2513211978858</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4">
+        <f>SUM(G27:G28)</f>
+        <v>1404.9289489136818</v>
+      </c>
+      <c r="H29" s="4">
+        <f>SUM(H27:H28)</f>
+        <v>9254.1855549031116</v>
+      </c>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4">
+        <f>G27/G23</f>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H31" s="4">
+        <f>H27/H23</f>
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I31" s="4">
+        <f>I27/I23</f>
+        <v>0.31880000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4">
+        <f>G28/G24</f>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H32" s="4">
+        <f>H28/H24</f>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="I32" s="4">
+        <f>I28/I24</f>
+        <v>0.31880000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4">
+        <f>G29/G25</f>
+        <v>0.31880000000000008</v>
+      </c>
+      <c r="H33" s="4">
+        <f>H29/H25</f>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="37" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="5">
+        <v>750</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1238</v>
+      </c>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="5">
+        <v>75</v>
+      </c>
+      <c r="D39" s="5">
+        <v>498</v>
+      </c>
+      <c r="E39" s="4">
+        <f>SUM(C38:D39)</f>
+        <v>2561</v>
+      </c>
+      <c r="F39">
+        <f>D39/C39</f>
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4">
+        <f>C39/C38</f>
+        <v>0.1</v>
+      </c>
+      <c r="D40" s="4">
+        <f>D39/D38</f>
+        <v>0.40226171243941844</v>
+      </c>
+      <c r="E40" s="4">
+        <f>D40/C40</f>
+        <v>4.0226171243941842</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="5">
+        <v>267</v>
+      </c>
+      <c r="D42" s="5">
+        <v>1721</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="5">
+        <v>21</v>
+      </c>
+      <c r="D43" s="5">
+        <v>552</v>
+      </c>
+      <c r="E43" s="4">
+        <f>SUM(C42:D43)</f>
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="5">
+        <v>881</v>
+      </c>
+      <c r="D46" s="5">
+        <v>1107</v>
+      </c>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="5">
+        <v>90</v>
+      </c>
+      <c r="D47" s="5">
+        <v>483</v>
+      </c>
+      <c r="E47" s="4">
+        <f>SUM(C46:D47)</f>
+        <v>2561</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{9C39114D-177D-874F-9648-8D0623AF7627}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Oversample by different oversampling factors
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Code/eliminating-bias-in-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A825C09-F476-7C4A-9212-72FD6313DA25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9F4E90-1737-B149-98E8-F4067E8CE1BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38680" yWindow="8280" windowWidth="37840" windowHeight="34860" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
   <si>
     <t>Training time</t>
   </si>
@@ -142,7 +142,10 @@
     <t>others</t>
   </si>
   <si>
-    <t>results</t>
+    <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=9duRaTjLSR25QcgMvYmERY</t>
+  </si>
+  <si>
+    <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=Qx6hSHQmgbTjyATwAUGogd</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -248,6 +251,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2818,9 +2822,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2829,179 +2835,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11">
+        <v>43501</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>43502</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1641</v>
-      </c>
-      <c r="H3" s="5">
-        <v>8305</v>
-      </c>
-      <c r="I3" s="4">
-        <f>SUM(G3:H3)</f>
-        <v>9946</v>
-      </c>
-      <c r="N3">
-        <f>N4/(N4+N5)</f>
-        <v>0.88618285679186759</v>
-      </c>
-      <c r="O3">
-        <f>M6/SUM(M6:M11)</f>
-        <v>0.8542735173981143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B4" s="4">
-        <f>SUM(G3:H4)</f>
-        <v>30000</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1777</v>
-      </c>
-      <c r="H4" s="5">
-        <v>18277</v>
-      </c>
-      <c r="I4" s="4">
-        <f>SUM(G4:H4)</f>
-        <v>20054</v>
-      </c>
-      <c r="N4">
-        <f>M6+M8</f>
-        <v>28855</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4">
-        <f>SUM(G3:G4)</f>
-        <v>3418</v>
-      </c>
-      <c r="H5" s="4">
-        <f>SUM(H3:H4)</f>
-        <v>26582</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="N5">
-        <f>M7+M9+M10</f>
-        <v>3706</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="I6" s="4"/>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="10">
-        <v>27816</v>
-      </c>
-      <c r="N6" s="8">
-        <f>M6/SUM($M$6:$M$10)</f>
-        <v>0.8542735173981143</v>
-      </c>
     </row>
     <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="5">
-        <v>101</v>
+        <v>1641</v>
       </c>
       <c r="H7" s="5">
-        <v>982</v>
+        <v>8305</v>
       </c>
       <c r="I7" s="4">
         <f>SUM(G7:H7)</f>
-        <v>1083</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="10">
-        <v>3124</v>
-      </c>
-      <c r="N7" s="8">
-        <f t="shared" ref="N7:N10" si="0">M7/SUM($M$6:$M$10)</f>
-        <v>9.5942999293633494E-2</v>
+        <v>9946</v>
+      </c>
+      <c r="N7">
+        <f>N8/(N8+N9)</f>
+        <v>0.88618285679186759</v>
+      </c>
+      <c r="O7">
+        <f>M10/SUM(M10:M15)</f>
+        <v>0.8542735173981143</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="B8" s="4">
+        <f>SUM(G7:H8)</f>
+        <v>30000</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="5">
-        <v>315</v>
+        <v>1777</v>
       </c>
       <c r="H8" s="5">
-        <v>5826</v>
+        <v>18277</v>
       </c>
       <c r="I8" s="4">
         <f>SUM(G8:H8)</f>
-        <v>6141</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="10">
-        <v>1039</v>
-      </c>
-      <c r="N8" s="8">
-        <f t="shared" si="0"/>
-        <v>3.1909339393753261E-2</v>
+        <v>20054</v>
+      </c>
+      <c r="N8">
+        <f>M10+M12</f>
+        <v>28855</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -3012,22 +2927,16 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4">
         <f>SUM(G7:G8)</f>
-        <v>416</v>
+        <v>3418</v>
       </c>
       <c r="H9" s="4">
         <f>SUM(H7:H8)</f>
-        <v>6808</v>
+        <v>26582</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="L9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="10">
-        <v>311</v>
-      </c>
-      <c r="N9" s="8">
-        <f t="shared" si="0"/>
-        <v>9.551303706888609E-3</v>
+      <c r="N9">
+        <f>M11+M13+M14</f>
+        <v>3706</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -3040,52 +2949,50 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="L10" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="M10" s="10">
-        <v>271</v>
+        <v>27816</v>
       </c>
       <c r="N10" s="8">
-        <f t="shared" si="0"/>
-        <v>8.3228402076103315E-3</v>
+        <f>M10/SUM($M$10:$M$14)</f>
+        <v>0.8542735173981143</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <f>G7/G3</f>
-        <v>6.1547836684948204E-2</v>
-      </c>
-      <c r="C11" s="4">
-        <f>H7/H3</f>
-        <v>0.11824202287778447</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="5">
-        <v>6.1499999999999999E-2</v>
+        <v>101</v>
       </c>
       <c r="H11" s="5">
-        <v>0.1182</v>
+        <v>982</v>
       </c>
       <c r="I11" s="4">
-        <f>I7/I3</f>
-        <v>0.10888799517393927</v>
+        <f>SUM(G11:H11)</f>
+        <v>1083</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="10">
+        <v>3124</v>
+      </c>
+      <c r="N11" s="8">
+        <f t="shared" ref="N11:N14" si="0">M11/SUM($M$10:$M$14)</f>
+        <v>9.5942999293633494E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
-        <f>G8/G4</f>
-        <v>0.17726505346088914</v>
-      </c>
-      <c r="C12" s="4">
-        <f>H8/H4</f>
-        <v>0.31876128467472781</v>
-      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
         <v>18</v>
@@ -3094,14 +3001,24 @@
         <v>24</v>
       </c>
       <c r="G12" s="5">
-        <v>0.17730000000000001</v>
+        <v>315</v>
       </c>
       <c r="H12" s="5">
-        <v>0.31879999999999997</v>
+        <v>5826</v>
       </c>
       <c r="I12" s="4">
-        <f>I8/I4</f>
-        <v>0.30622319736710879</v>
+        <f>SUM(G12:H12)</f>
+        <v>6141</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="10">
+        <v>1039</v>
+      </c>
+      <c r="N12" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1909339393753261E-2</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -3111,14 +3028,24 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4">
-        <f>G9/G5</f>
-        <v>0.12170860152135751</v>
+        <f>SUM(G11:G12)</f>
+        <v>416</v>
       </c>
       <c r="H13" s="4">
-        <f>H9/H5</f>
-        <v>0.25611315928071626</v>
+        <f>SUM(H11:H12)</f>
+        <v>6808</v>
       </c>
       <c r="I13" s="4"/>
+      <c r="L13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="10">
+        <v>311</v>
+      </c>
+      <c r="N13" s="8">
+        <f t="shared" si="0"/>
+        <v>9.551303706888609E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
@@ -3129,65 +3056,90 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="L14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="10">
+        <v>271</v>
+      </c>
+      <c r="N14" s="8">
+        <f t="shared" si="0"/>
+        <v>8.3228402076103315E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <f>G11/G7</f>
+        <v>6.1547836684948204E-2</v>
+      </c>
+      <c r="C15" s="4">
+        <f>H11/H7</f>
+        <v>0.11824202287778447</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4">
-        <f>$H$12/G11</f>
-        <v>5.1837398373983739</v>
-      </c>
-      <c r="H15" s="4">
-        <f>$H$12/H11</f>
-        <v>2.6971235194585446</v>
+        <v>19</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="5">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.1182</v>
       </c>
       <c r="I15" s="4">
-        <f>I12/I11</f>
-        <v>2.8122769353769752</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+        <f>I11/I7</f>
+        <v>0.10888799517393927</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <f>G12/G8</f>
+        <v>0.17726505346088914</v>
+      </c>
+      <c r="C16" s="4">
+        <f>H12/H8</f>
+        <v>0.31876128467472781</v>
+      </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4">
-        <f>$H$12/G12</f>
-        <v>1.7980823463056963</v>
-      </c>
-      <c r="H16" s="4">
-        <f>$H$12/H12</f>
-        <v>1</v>
-      </c>
-      <c r="I16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.17730000000000001</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I16" s="4">
+        <f>I12/I8</f>
+        <v>0.30622319736710879</v>
+      </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>619.58789999999999</v>
-      </c>
-      <c r="C17">
-        <v>2444.5385999999999</v>
-      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4">
+        <f>G13/G9</f>
+        <v>0.12170860152135751</v>
+      </c>
       <c r="H17" s="4">
-        <f>H13/G13</f>
-        <v>2.1043143712055006</v>
+        <f>H13/H9</f>
+        <v>0.25611315928071626</v>
       </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <v>369.09059999999999</v>
-      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -3196,60 +3148,63 @@
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="4">
-        <v>422.55772357723578</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1666.5752961082908</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4">
-        <f>($H$12*G3 - G7)/(1 - $H$12)</f>
-        <v>619.71638285378742</v>
+        <f>$H$16/G15</f>
+        <v>5.1837398373983739</v>
       </c>
       <c r="H19" s="4">
-        <f>($H$12*H3-H7)/(1-$H$12)</f>
-        <v>2445.1467997651198</v>
-      </c>
-      <c r="I19" s="4"/>
+        <f>$H$16/H15</f>
+        <v>2.6971235194585446</v>
+      </c>
+      <c r="I19" s="4">
+        <f>I16/I15</f>
+        <v>2.8122769353769752</v>
+      </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="4">
-        <v>251.39593908629433</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4">
-        <f>($H$12*G4-G8)/(1-$H$12)</f>
-        <v>369.21256605989419</v>
+        <f>$H$16/G16</f>
+        <v>1.7980823463056963</v>
       </c>
       <c r="H20" s="4">
-        <f>($H$12*H4-H8)/(1-$H$12)</f>
-        <v>1.0387551379913817</v>
+        <f>$H$16/H16</f>
+        <v>1</v>
       </c>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21">
+        <v>619.58789999999999</v>
+      </c>
+      <c r="C21">
+        <v>2444.5385999999999</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4">
+        <f>H17/G17</f>
+        <v>2.1043143712055006</v>
+      </c>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="B22">
+        <v>369.09059999999999</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -3258,44 +3213,46 @@
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="4">
+        <v>422.55772357723578</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1666.5752961082908</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4">
-        <f>G3+G19</f>
-        <v>2260.7163828537873</v>
+        <f>($H$16*G7 - G11)/(1 - $H$16)</f>
+        <v>619.71638285378742</v>
       </c>
       <c r="H23" s="4">
-        <f>H3+H19</f>
-        <v>10750.14679976512</v>
-      </c>
-      <c r="I23" s="4">
-        <f>SUM(G23:H23)</f>
-        <v>13010.863182618907</v>
-      </c>
+        <f>($H$16*H7-H11)/(1-$H$16)</f>
+        <v>2445.1467997651198</v>
+      </c>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="B24" s="4">
+        <v>251.39593908629433</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4">
-        <f>G4+G20</f>
-        <v>2146.212566059894</v>
+        <f>($H$16*G8-G12)/(1-$H$16)</f>
+        <v>369.21256605989419</v>
       </c>
       <c r="H24" s="4">
-        <f>H4+H20</f>
-        <v>18278.03875513799</v>
-      </c>
-      <c r="I24" s="4">
-        <f>SUM(G24:H24)</f>
-        <v>20424.251321197884</v>
-      </c>
+        <f>($H$16*H8-H12)/(1-$H$16)</f>
+        <v>1.0387551379913817</v>
+      </c>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
@@ -3303,14 +3260,8 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="4">
-        <f>SUM(G23:G24)</f>
-        <v>4406.9289489136809</v>
-      </c>
-      <c r="H25" s="4">
-        <f>SUM(H23:H24)</f>
-        <v>29028.18555490311</v>
-      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
@@ -3324,57 +3275,43 @@
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="4">
-        <f>G15*G7</f>
-        <v>523.55772357723572</v>
-      </c>
-      <c r="C27" s="4">
-        <f>H15*H7</f>
-        <v>2648.5752961082908</v>
-      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4">
-        <f>G19+G7</f>
-        <v>720.71638285378742</v>
+        <f>G7+G23</f>
+        <v>2260.7163828537873</v>
       </c>
       <c r="H27" s="4">
-        <f>H19+H7</f>
-        <v>3427.1467997651198</v>
+        <f>H7+H23</f>
+        <v>10750.14679976512</v>
       </c>
       <c r="I27" s="4">
         <f>SUM(G27:H27)</f>
-        <v>4147.8631826189076</v>
+        <v>13010.863182618907</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="4">
-        <f>G16*G8</f>
-        <v>566.39593908629433</v>
-      </c>
-      <c r="C28" s="4">
-        <f>H16*H8</f>
-        <v>5826</v>
-      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4">
-        <f>G20+G8</f>
-        <v>684.21256605989424</v>
+        <f>G8+G24</f>
+        <v>2146.212566059894</v>
       </c>
       <c r="H28" s="4">
-        <f>H20+H8</f>
-        <v>5827.0387551379918</v>
+        <f>H8+H24</f>
+        <v>18278.03875513799</v>
       </c>
       <c r="I28" s="4">
         <f>SUM(G28:H28)</f>
-        <v>6511.2513211978858</v>
+        <v>20424.251321197884</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
@@ -3385,11 +3322,11 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4">
         <f>SUM(G27:G28)</f>
-        <v>1404.9289489136818</v>
+        <v>4406.9289489136809</v>
       </c>
       <c r="H29" s="4">
         <f>SUM(H27:H28)</f>
-        <v>9254.1855549031116</v>
+        <v>29028.18555490311</v>
       </c>
       <c r="I29" s="4"/>
     </row>
@@ -3404,45 +3341,57 @@
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="4">
+        <f>G19*G11</f>
+        <v>523.55772357723572</v>
+      </c>
+      <c r="C31" s="4">
+        <f>H19*H11</f>
+        <v>2648.5752961082908</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4">
-        <f>G27/G23</f>
-        <v>0.31880000000000003</v>
+        <f>G23+G11</f>
+        <v>720.71638285378742</v>
       </c>
       <c r="H31" s="4">
-        <f>H27/H23</f>
-        <v>0.31879999999999997</v>
+        <f>H23+H11</f>
+        <v>3427.1467997651198</v>
       </c>
       <c r="I31" s="4">
-        <f>I27/I23</f>
-        <v>0.31880000000000003</v>
+        <f>SUM(G31:H31)</f>
+        <v>4147.8631826189076</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="4">
+        <f>G20*G12</f>
+        <v>566.39593908629433</v>
+      </c>
+      <c r="C32" s="4">
+        <f>H20*H12</f>
+        <v>5826</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4">
-        <f>G28/G24</f>
-        <v>0.31880000000000003</v>
+        <f>G24+G12</f>
+        <v>684.21256605989424</v>
       </c>
       <c r="H32" s="4">
-        <f>H28/H24</f>
-        <v>0.31880000000000003</v>
+        <f>H24+H12</f>
+        <v>5827.0387551379918</v>
       </c>
       <c r="I32" s="4">
-        <f>I28/I24</f>
-        <v>0.31880000000000003</v>
+        <f>SUM(G32:H32)</f>
+        <v>6511.2513211978858</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
@@ -3452,78 +3401,90 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4">
-        <f>G29/G25</f>
+        <f>SUM(G31:G32)</f>
+        <v>1404.9289489136818</v>
+      </c>
+      <c r="H33" s="4">
+        <f>SUM(H31:H32)</f>
+        <v>9254.1855549031116</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4">
+        <f t="shared" ref="G35:I36" si="1">G31/G27</f>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I35" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31880000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H36" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="I36" s="4">
+        <f t="shared" si="1"/>
+        <v>0.31880000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4">
+        <f>G33/G29</f>
         <v>0.31880000000000008</v>
       </c>
-      <c r="H33" s="4">
-        <f>H29/H25</f>
+      <c r="H37" s="4">
+        <f>H33/H29</f>
         <v>0.31880000000000003</v>
       </c>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="37" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
-      <c r="C37" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="5">
-        <v>750</v>
-      </c>
-      <c r="D38" s="5">
-        <v>1238</v>
-      </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="5">
-        <v>75</v>
-      </c>
-      <c r="D39" s="5">
-        <v>498</v>
-      </c>
-      <c r="E39" s="4">
-        <f>SUM(C38:D39)</f>
-        <v>2561</v>
-      </c>
-      <c r="F39">
-        <f>D39/C39</f>
-        <v>6.64</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="4"/>
-      <c r="C40" s="4">
-        <f>C39/C38</f>
-        <v>0.1</v>
-      </c>
-      <c r="D40" s="4">
-        <f>D39/D38</f>
-        <v>0.40226171243941844</v>
-      </c>
-      <c r="E40" s="4">
-        <f>D40/C40</f>
-        <v>4.0226171243941842</v>
-      </c>
+      <c r="I37" s="4"/>
     </row>
     <row r="41" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E41" s="4"/>
     </row>
@@ -3532,10 +3493,10 @@
         <v>34</v>
       </c>
       <c r="C42" s="5">
-        <v>267</v>
+        <v>750</v>
       </c>
       <c r="D42" s="5">
-        <v>1721</v>
+        <v>1238</v>
       </c>
       <c r="E42" s="4"/>
     </row>
@@ -3544,29 +3505,42 @@
         <v>18</v>
       </c>
       <c r="C43" s="5">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="D43" s="5">
-        <v>552</v>
+        <v>498</v>
       </c>
       <c r="E43" s="4">
         <f>SUM(C42:D43)</f>
         <v>2561</v>
       </c>
+      <c r="F43">
+        <f>D43/C43</f>
+        <v>6.64</v>
+      </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
+      <c r="C44" s="4">
+        <f>C43/C42</f>
+        <v>0.1</v>
+      </c>
+      <c r="D44" s="4">
+        <f>D43/D42</f>
+        <v>0.40226171243941844</v>
+      </c>
+      <c r="E44" s="4">
+        <f>D44/C44</f>
+        <v>4.0226171243941842</v>
+      </c>
     </row>
     <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
       <c r="C45" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E45" s="4"/>
     </row>
@@ -3575,10 +3549,10 @@
         <v>34</v>
       </c>
       <c r="C46" s="5">
-        <v>881</v>
+        <v>267</v>
       </c>
       <c r="D46" s="5">
-        <v>1107</v>
+        <v>1721</v>
       </c>
       <c r="E46" s="4"/>
     </row>
@@ -3587,19 +3561,63 @@
         <v>18</v>
       </c>
       <c r="C47" s="5">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="D47" s="5">
-        <v>483</v>
+        <v>552</v>
       </c>
       <c r="E47" s="4">
         <f>SUM(C46:D47)</f>
         <v>2561</v>
       </c>
     </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="5">
+        <v>881</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1107</v>
+      </c>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="5">
+        <v>90</v>
+      </c>
+      <c r="D51" s="5">
+        <v>483</v>
+      </c>
+      <c r="E51" s="4">
+        <f>SUM(C50:D51)</f>
+        <v>2561</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{9C39114D-177D-874F-9648-8D0623AF7627}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{9C39114D-177D-874F-9648-8D0623AF7627}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{62BC5D29-BC2E-BE4F-9971-6E1802D9851C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Make successive results pngs for presentation gif
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -2,24 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Code/eliminating-bias-in-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9F4E90-1737-B149-98E8-F4067E8CE1BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA0A014-5276-824A-8195-C487F1B9CAC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="46080" yWindow="10420" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
     <sheet name="Gender &amp; Race" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="Performance Metrics" sheetId="3" r:id="rId4"/>
+    <sheet name="Pie Charts" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet2!$B$10:$G$18</definedName>
     <definedName name="row">Gender!$B$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
   <si>
     <t>Training time</t>
   </si>
@@ -147,12 +152,57 @@
   <si>
     <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=Qx6hSHQmgbTjyATwAUGogd</t>
   </si>
+  <si>
+    <t>GANs</t>
+  </si>
+  <si>
+    <t>Oversampling</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Am-In-Es</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>F1 score</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Oversample Factor</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Training Iterations</t>
+  </si>
+  <si>
+    <t>Bias Factors</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +264,47 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF101620"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF101620"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,12 +314,64 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -237,7 +380,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -252,6 +395,41 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -271,10 +449,1753 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pie Charts'!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Male</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Female</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pie Charts'!$C$1:$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>27816</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10771</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4EB8-B242-9623-5A8E71F44363}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="3600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-322F-2244-8144-5AF1AC7E2413}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-322F-2244-8144-5AF1AC7E2413}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pie Charts'!$B$5:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>White</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Black</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Asian</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Am-In-Es</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pie Charts'!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>27816</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1039</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>271</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-322F-2244-8144-5AF1AC7E2413}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A4166D1-300F-754B-8B18-84A574B5E9F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADD506B0-E288-ED40-A347-D453158406E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Blue Green">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -282,34 +2203,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="373545"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="CEDBE6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="3494BA"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="58B6C0"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="75BDA7"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="7A8C8E"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="84ACB6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="2683C6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="6B9F25"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="9F6715"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -571,7 +2492,7 @@
   <dimension ref="B2:M134"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L96" sqref="L96"/>
+      <selection activeCell="C9" sqref="C9:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2816,7 +4737,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2824,7 +4745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2986,7 +4907,7 @@
         <v>3124</v>
       </c>
       <c r="N11" s="8">
-        <f t="shared" ref="N11:N14" si="0">M11/SUM($M$10:$M$14)</f>
+        <f>M11/SUM($M$10:$M$14)</f>
         <v>9.5942999293633494E-2</v>
       </c>
     </row>
@@ -3017,7 +4938,7 @@
         <v>1039</v>
       </c>
       <c r="N12" s="8">
-        <f t="shared" si="0"/>
+        <f>M12/SUM($M$10:$M$14)</f>
         <v>3.1909339393753261E-2</v>
       </c>
     </row>
@@ -3043,7 +4964,7 @@
         <v>311</v>
       </c>
       <c r="N13" s="8">
-        <f t="shared" si="0"/>
+        <f>M13/SUM($M$10:$M$14)</f>
         <v>9.551303706888609E-3</v>
       </c>
     </row>
@@ -3063,7 +4984,7 @@
         <v>271</v>
       </c>
       <c r="N14" s="8">
-        <f t="shared" si="0"/>
+        <f>M14/SUM($M$10:$M$14)</f>
         <v>8.3228402076103315E-3</v>
       </c>
     </row>
@@ -3429,15 +5350,15 @@
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4">
-        <f t="shared" ref="G35:I36" si="1">G31/G27</f>
+        <f t="shared" ref="G35:I36" si="0">G31/G27</f>
         <v>0.31880000000000003</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.31879999999999997</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.31880000000000003</v>
       </c>
     </row>
@@ -3450,15 +5371,15 @@
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.31880000000000003</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.31880000000000003</v>
       </c>
       <c r="I36" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.31880000000000003</v>
       </c>
     </row>
@@ -3621,4 +5542,536 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6489FE5E-6E3D-FF41-8AE5-CA5D9359547D}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B9:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="31">
+        <v>5</v>
+      </c>
+      <c r="F11" s="31">
+        <v>162</v>
+      </c>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="26">
+        <v>0.86</v>
+      </c>
+      <c r="E13" s="26">
+        <v>0.83</v>
+      </c>
+      <c r="F13" s="26">
+        <v>0.83</v>
+      </c>
+      <c r="G13" s="26">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="21"/>
+      <c r="C14" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="27">
+        <v>0.69</v>
+      </c>
+      <c r="E14" s="27">
+        <v>0.65</v>
+      </c>
+      <c r="F14" s="27">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G14" s="27">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="21"/>
+      <c r="C15" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="27">
+        <v>0.71</v>
+      </c>
+      <c r="E15" s="27">
+        <v>0.63</v>
+      </c>
+      <c r="F15" s="27">
+        <v>0.73</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0.67</v>
+      </c>
+      <c r="E16" s="28">
+        <v>0.67</v>
+      </c>
+      <c r="F16" s="28">
+        <v>0.46</v>
+      </c>
+      <c r="G16" s="28">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="29">
+        <v>2.79</v>
+      </c>
+      <c r="E17" s="29">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F17" s="29">
+        <v>1.25</v>
+      </c>
+      <c r="G17" s="29">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+      <c r="C18" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="30">
+        <v>2.8</v>
+      </c>
+      <c r="E18" s="32">
+        <v>1.21</v>
+      </c>
+      <c r="F18" s="32">
+        <v>1.04</v>
+      </c>
+      <c r="G18" s="32">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C05B230-2BFF-B143-9BA5-EBAB290E553A}">
+  <dimension ref="E7:L22"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="F7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="5:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13">
+        <v>10000</v>
+      </c>
+      <c r="K10" s="13">
+        <v>20000</v>
+      </c>
+      <c r="L10" s="13">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="11" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="14">
+        <v>23.684200000000001</v>
+      </c>
+      <c r="K11" s="14">
+        <v>43.596699999999998</v>
+      </c>
+      <c r="L11" s="14">
+        <v>79.695300000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="14">
+        <v>9.4600000000000004E-2</v>
+      </c>
+      <c r="K12" s="14">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="L12" s="14">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="14">
+        <v>0.71230000000000004</v>
+      </c>
+      <c r="K13" s="14">
+        <v>0.7117</v>
+      </c>
+      <c r="L13" s="14">
+        <v>0.71309999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0.66090000000000004</v>
+      </c>
+      <c r="K14" s="14">
+        <v>0.67130000000000001</v>
+      </c>
+      <c r="L14" s="14">
+        <v>0.67079999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0.79110000000000003</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0.78559999999999997</v>
+      </c>
+      <c r="L15" s="14">
+        <v>0.79379999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0.7087</v>
+      </c>
+      <c r="K16" s="14">
+        <v>0.72419999999999995</v>
+      </c>
+      <c r="L16" s="14">
+        <v>0.72950000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="14">
+        <v>0.64780000000000004</v>
+      </c>
+      <c r="K17" s="14">
+        <v>0.65049999999999997</v>
+      </c>
+      <c r="L17" s="14">
+        <v>0.64729999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="14">
+        <v>0.61909999999999998</v>
+      </c>
+      <c r="K18" s="14">
+        <v>0.62560000000000004</v>
+      </c>
+      <c r="L18" s="14">
+        <v>0.62070000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="14">
+        <v>0.874</v>
+      </c>
+      <c r="K19" s="14">
+        <v>0.87309999999999999</v>
+      </c>
+      <c r="L19" s="14">
+        <v>0.87460000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="I20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="14">
+        <v>0.84689999999999999</v>
+      </c>
+      <c r="K20" s="14">
+        <v>0.85240000000000005</v>
+      </c>
+      <c r="L20" s="14">
+        <v>0.85319999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="I21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="14">
+        <v>0.93389999999999995</v>
+      </c>
+      <c r="K21" s="14">
+        <v>0.93289999999999995</v>
+      </c>
+      <c r="L21" s="14">
+        <v>0.93279999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="I22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="14">
+        <v>0.90610000000000002</v>
+      </c>
+      <c r="K22" s="14">
+        <v>0.91220000000000001</v>
+      </c>
+      <c r="L22" s="14">
+        <v>0.91279999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7BED9A-409F-B04C-A0A7-4BF7B624C54C}">
+  <dimension ref="B1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="15">
+        <v>27816</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="15">
+        <v>10771</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="16"/>
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="16"/>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="15">
+        <v>27816</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="15">
+        <v>3124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="15">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="15">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="15">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update plots for slides and reorganise figures
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,26 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Code/eliminating-bias-in-ml/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Code/debias-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA0A014-5276-824A-8195-C487F1B9CAC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE77D57-1B70-E04C-9B08-75AC162CC0EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46080" yWindow="10420" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
     <sheet name="Gender &amp; Race" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
-    <sheet name="Performance Metrics" sheetId="3" r:id="rId4"/>
-    <sheet name="Pie Charts" sheetId="4" r:id="rId5"/>
+    <sheet name="Comparison with GANs" sheetId="5" r:id="rId3"/>
+    <sheet name="Pie Charts" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet2!$B$10:$G$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Comparison with GANs'!$B$10:$H$18</definedName>
     <definedName name="row">Gender!$B$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="60">
   <si>
     <t>Training time</t>
   </si>
@@ -196,13 +194,31 @@
   </si>
   <si>
     <t>Bias Factors</t>
+  </si>
+  <si>
+    <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=8YJwqUhK1jSHPi6TkpQ9</t>
+  </si>
+  <si>
+    <t>Bias</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=X8MmNyfWPSPUjmg4psrjBM</t>
+  </si>
+  <si>
+    <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=HpMQLQaCFmL4p2dgA86Wz9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -265,26 +281,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF101620"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF101620"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -314,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -374,13 +370,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="double">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -396,18 +405,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -416,20 +422,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -529,6 +539,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-97F3-3244-8624-D1E0D9FDD80C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -549,6 +564,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-97F3-3244-8624-D1E0D9FDD80C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -808,6 +828,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-4CF2-134F-9685-EAA76E5F5262}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -828,6 +853,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-4CF2-134F-9685-EAA76E5F5262}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -848,6 +878,11 @@
                 </a:contourClr>
               </a:sp3d>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-4CF2-134F-9685-EAA76E5F5262}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4745,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4771,6 +4806,30 @@
         <v>37</v>
       </c>
     </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>43503</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>43506</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
+        <v>43507</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="6" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -5539,6 +5598,9 @@
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{9C39114D-177D-874F-9648-8D0623AF7627}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{62BC5D29-BC2E-BE4F-9971-6E1802D9851C}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{B88AF874-80B7-F843-B08B-3A0D063425A5}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{A5515785-4094-994E-9541-747616D5BC0D}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{62FEC5B1-56D8-7740-8ED0-F73ED66D809E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5549,174 +5611,201 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B9:G19"/>
+  <dimension ref="B9:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:G18"/>
+    <sheetView topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="4" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="25" t="s">
+    <row r="9" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="G10" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="31">
-        <v>5</v>
-      </c>
-      <c r="F11" s="31">
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="28">
+        <v>6</v>
+      </c>
+      <c r="G11" s="28">
         <v>162</v>
       </c>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="2:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="25" t="s">
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="F12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="G12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="H12" s="22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="20" t="s">
+    <row r="13" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="26">
+        <v>2.8</v>
+      </c>
+      <c r="E13" s="26">
+        <v>3.16</v>
+      </c>
+      <c r="F13" s="26">
+        <v>1.19</v>
+      </c>
+      <c r="G13" s="26">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H13" s="26">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+      <c r="C14" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="27">
+        <v>2.99</v>
+      </c>
+      <c r="E14" s="27">
+        <v>2.59</v>
+      </c>
+      <c r="F14" s="29">
+        <v>1.24</v>
+      </c>
+      <c r="G14" s="29">
+        <v>1.04</v>
+      </c>
+      <c r="H14" s="29">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C15" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D15" s="23">
         <v>0.86</v>
       </c>
-      <c r="E13" s="26">
-        <v>0.83</v>
-      </c>
-      <c r="F13" s="26">
-        <v>0.83</v>
-      </c>
-      <c r="G13" s="26">
+      <c r="E15" s="23">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="21"/>
-      <c r="C14" s="23" t="s">
+      <c r="F15" s="23">
+        <v>0.82</v>
+      </c>
+      <c r="G15" s="23">
+        <v>0.82</v>
+      </c>
+      <c r="H15" s="23">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="18"/>
+      <c r="C16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D16" s="24">
         <v>0.69</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E16" s="24">
+        <v>0.69</v>
+      </c>
+      <c r="F16" s="24">
         <v>0.65</v>
       </c>
-      <c r="F14" s="27">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G14" s="27">
+      <c r="G16" s="24">
+        <v>0.48</v>
+      </c>
+      <c r="H16" s="24">
         <v>0.69</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="21"/>
-      <c r="C15" s="23" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="27">
-        <v>0.71</v>
-      </c>
-      <c r="E15" s="27">
-        <v>0.63</v>
-      </c>
-      <c r="F15" s="27">
-        <v>0.73</v>
-      </c>
-      <c r="G15" s="27">
+      <c r="D17" s="24">
+        <v>0.72</v>
+      </c>
+      <c r="E17" s="24">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="24" t="s">
+      <c r="F17" s="24">
+        <v>0.62</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0.78</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="19"/>
+      <c r="C18" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="28">
-        <v>0.67</v>
-      </c>
-      <c r="E16" s="28">
-        <v>0.67</v>
-      </c>
-      <c r="F16" s="28">
-        <v>0.46</v>
-      </c>
-      <c r="G16" s="28">
+      <c r="D18" s="25">
+        <v>0.66</v>
+      </c>
+      <c r="E18" s="25">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="29">
-        <v>2.79</v>
-      </c>
-      <c r="E17" s="29">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="F17" s="29">
-        <v>1.25</v>
-      </c>
-      <c r="G17" s="29">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
-      <c r="C18" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="30">
-        <v>2.8</v>
-      </c>
-      <c r="E18" s="32">
-        <v>1.21</v>
-      </c>
-      <c r="F18" s="32">
-        <v>1.04</v>
-      </c>
-      <c r="G18" s="32">
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="F18" s="25">
+        <v>0.69</v>
+      </c>
+      <c r="G18" s="25">
+        <v>0.35</v>
+      </c>
+      <c r="H18" s="25">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5724,349 +5813,79 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C05B230-2BFF-B143-9BA5-EBAB290E553A}">
-  <dimension ref="E7:L22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7BED9A-409F-B04C-A0A7-4BF7B624C54C}">
+  <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15" customWidth="1"/>
-    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="F7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="5:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13">
-        <v>10000</v>
-      </c>
-      <c r="K10" s="13">
-        <v>20000</v>
-      </c>
-      <c r="L10" s="13">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="11" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="14">
-        <v>23.684200000000001</v>
-      </c>
-      <c r="K11" s="14">
-        <v>43.596699999999998</v>
-      </c>
-      <c r="L11" s="14">
-        <v>79.695300000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="14">
-        <v>9.4600000000000004E-2</v>
-      </c>
-      <c r="K12" s="14">
-        <v>4.0899999999999999E-2</v>
-      </c>
-      <c r="L12" s="14">
-        <v>5.8999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="14">
-        <v>0.71230000000000004</v>
-      </c>
-      <c r="K13" s="14">
-        <v>0.7117</v>
-      </c>
-      <c r="L13" s="14">
-        <v>0.71309999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="14">
-        <v>0.66090000000000004</v>
-      </c>
-      <c r="K14" s="14">
-        <v>0.67130000000000001</v>
-      </c>
-      <c r="L14" s="14">
-        <v>0.67079999999999995</v>
-      </c>
-    </row>
-    <row r="15" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="14">
-        <v>0.79110000000000003</v>
-      </c>
-      <c r="K15" s="14">
-        <v>0.78559999999999997</v>
-      </c>
-      <c r="L15" s="14">
-        <v>0.79379999999999995</v>
-      </c>
-    </row>
-    <row r="16" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" s="14">
-        <v>0.7087</v>
-      </c>
-      <c r="K16" s="14">
-        <v>0.72419999999999995</v>
-      </c>
-      <c r="L16" s="14">
-        <v>0.72950000000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="14">
-        <v>0.64780000000000004</v>
-      </c>
-      <c r="K17" s="14">
-        <v>0.65049999999999997</v>
-      </c>
-      <c r="L17" s="14">
-        <v>0.64729999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="14">
-        <v>0.61909999999999998</v>
-      </c>
-      <c r="K18" s="14">
-        <v>0.62560000000000004</v>
-      </c>
-      <c r="L18" s="14">
-        <v>0.62070000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="E19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="14">
-        <v>0.874</v>
-      </c>
-      <c r="K19" s="14">
-        <v>0.87309999999999999</v>
-      </c>
-      <c r="L19" s="14">
-        <v>0.87460000000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="I20" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="14">
-        <v>0.84689999999999999</v>
-      </c>
-      <c r="K20" s="14">
-        <v>0.85240000000000005</v>
-      </c>
-      <c r="L20" s="14">
-        <v>0.85319999999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="I21" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" s="14">
-        <v>0.93389999999999995</v>
-      </c>
-      <c r="K21" s="14">
-        <v>0.93289999999999995</v>
-      </c>
-      <c r="L21" s="14">
-        <v>0.93279999999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="5:12" ht="18" x14ac:dyDescent="0.25">
-      <c r="I22" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" s="14">
-        <v>0.90610000000000002</v>
-      </c>
-      <c r="K22" s="14">
-        <v>0.91220000000000001</v>
-      </c>
-      <c r="L22" s="14">
-        <v>0.91279999999999994</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7BED9A-409F-B04C-A0A7-4BF7B624C54C}">
-  <dimension ref="B1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="10.83203125" style="17"/>
+    <col min="2" max="2" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="15">
+      <c r="C1" s="12">
         <v>27816</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="12">
         <v>10771</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="16"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>27816</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>3124</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>1039</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>311</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>271</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update README.md and reorganise figures
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Code/debias-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE77D57-1B70-E04C-9B08-75AC162CC0EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38BA8B7-3949-F443-BB26-F379884CC645}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="7420" yWindow="7240" windowWidth="26180" windowHeight="13760" activeTab="2" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Pie Charts" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Comparison with GANs'!$B$10:$H$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Comparison with GANs'!$B$2:$H$10</definedName>
     <definedName name="row">Gender!$B$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -4780,7 +4780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -5611,10 +5611,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B9:H19"/>
+  <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5625,187 +5625,187 @@
     <col min="8" max="8" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="32" t="s">
+    <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="22" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="33" t="s">
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="28">
-        <v>6</v>
-      </c>
-      <c r="G11" s="28">
-        <v>162</v>
-      </c>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="31" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="28">
+        <v>5</v>
+      </c>
+      <c r="G3" s="28">
+        <v>165</v>
+      </c>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F4" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H4" s="22" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="17" t="s">
+    <row r="5" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C5" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="26">
-        <v>2.8</v>
-      </c>
-      <c r="E13" s="26">
-        <v>3.16</v>
-      </c>
-      <c r="F13" s="26">
+      <c r="D5" s="26">
+        <v>2.92</v>
+      </c>
+      <c r="E5" s="26">
+        <v>2.79</v>
+      </c>
+      <c r="F5" s="26">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="G5" s="26">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H5" s="26">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="27">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E6" s="27">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F6" s="29">
         <v>1.19</v>
       </c>
-      <c r="G13" s="26">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="H13" s="26">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="27">
-        <v>2.99</v>
-      </c>
-      <c r="E14" s="27">
-        <v>2.59</v>
-      </c>
-      <c r="F14" s="29">
-        <v>1.24</v>
-      </c>
-      <c r="G14" s="29">
+      <c r="G6" s="29">
         <v>1.04</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H6" s="29">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="17" t="s">
+    <row r="7" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D7" s="23">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.85</v>
+      </c>
+      <c r="F7" s="23">
+        <v>0.83</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.82</v>
+      </c>
+      <c r="H7" s="23">
         <v>0.86</v>
       </c>
-      <c r="E15" s="23">
-        <v>0.86</v>
-      </c>
-      <c r="F15" s="23">
-        <v>0.82</v>
-      </c>
-      <c r="G15" s="23">
-        <v>0.82</v>
-      </c>
-      <c r="H15" s="23">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="18"/>
-      <c r="C16" s="20" t="s">
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="18"/>
+      <c r="C8" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D8" s="24">
+        <v>0.67</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.67</v>
+      </c>
+      <c r="F8" s="24">
+        <v>0.65</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0.48</v>
+      </c>
+      <c r="H8" s="24">
         <v>0.69</v>
       </c>
-      <c r="E16" s="24">
-        <v>0.69</v>
-      </c>
-      <c r="F16" s="24">
-        <v>0.65</v>
-      </c>
-      <c r="G16" s="24">
-        <v>0.48</v>
-      </c>
-      <c r="H16" s="24">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="18"/>
-      <c r="C17" s="20" t="s">
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="18"/>
+      <c r="C9" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D9" s="24">
         <v>0.72</v>
       </c>
-      <c r="E17" s="24">
-        <v>0.74</v>
-      </c>
-      <c r="F17" s="24">
+      <c r="E9" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="F9" s="24">
+        <v>0.64</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0.78</v>
+      </c>
+      <c r="H9" s="24">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="25">
         <v>0.62</v>
       </c>
-      <c r="G17" s="24">
-        <v>0.78</v>
-      </c>
-      <c r="H17" s="24">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="25">
+      <c r="E10" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="25">
+        <v>0.67</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0.35</v>
+      </c>
+      <c r="H10" s="25">
         <v>0.66</v>
       </c>
-      <c r="E18" s="25">
-        <v>0.64</v>
-      </c>
-      <c r="F18" s="25">
-        <v>0.69</v>
-      </c>
-      <c r="G18" s="25">
-        <v>0.35</v>
-      </c>
-      <c r="H18" s="25">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="11" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update READMEs and tidy up files
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Code/debias-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38BA8B7-3949-F443-BB26-F379884CC645}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD400838-AD8D-3F49-B025-6D8DBFFD8C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="7240" windowWidth="26180" windowHeight="13760" activeTab="2" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="7420" yWindow="7240" windowWidth="26180" windowHeight="13760" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
   <si>
     <t>Training time</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=HpMQLQaCFmL4p2dgA86Wz9</t>
+  </si>
+  <si>
+    <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=2vHQ1bySr6a1FnzM6x14De</t>
   </si>
 </sst>
 </file>
@@ -4778,10 +4781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D3" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4830,93 +4833,81 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>43513</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1641</v>
-      </c>
-      <c r="H7" s="5">
-        <v>8305</v>
-      </c>
-      <c r="I7" s="4">
-        <f>SUM(G7:H7)</f>
-        <v>9946</v>
-      </c>
-      <c r="N7">
-        <f>N8/(N8+N9)</f>
-        <v>0.88618285679186759</v>
-      </c>
-      <c r="O7">
-        <f>M10/SUM(M10:M15)</f>
-        <v>0.8542735173981143</v>
-      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <f>SUM(G7:H8)</f>
-        <v>30000</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" s="5">
-        <v>1777</v>
+        <v>1641</v>
       </c>
       <c r="H8" s="5">
-        <v>18277</v>
+        <v>8305</v>
       </c>
       <c r="I8" s="4">
         <f>SUM(G8:H8)</f>
-        <v>20054</v>
+        <v>9946</v>
       </c>
       <c r="N8">
-        <f>M10+M12</f>
-        <v>28855</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
+        <f>N9/(N9+N10)</f>
+        <v>0.88618285679186759</v>
+      </c>
+      <c r="O8">
+        <f>M11/SUM(M11:M16)</f>
+        <v>0.8542735173981143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <f>SUM(G8:H9)</f>
+        <v>30000</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4">
-        <f>SUM(G7:G8)</f>
-        <v>3418</v>
-      </c>
-      <c r="H9" s="4">
-        <f>SUM(H7:H8)</f>
-        <v>26582</v>
-      </c>
-      <c r="I9" s="4"/>
+      <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1777</v>
+      </c>
+      <c r="H9" s="5">
+        <v>18277</v>
+      </c>
+      <c r="I9" s="4">
+        <f>SUM(G9:H9)</f>
+        <v>20054</v>
+      </c>
       <c r="N9">
-        <f>M11+M13+M14</f>
-        <v>3706</v>
+        <f>M11+M13</f>
+        <v>28855</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -4925,49 +4916,38 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="G10" s="4">
+        <f>SUM(G8:G9)</f>
+        <v>3418</v>
+      </c>
+      <c r="H10" s="4">
+        <f>SUM(H8:H9)</f>
+        <v>26582</v>
+      </c>
       <c r="I10" s="4"/>
-      <c r="L10" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="10">
-        <v>27816</v>
-      </c>
-      <c r="N10" s="8">
-        <f>M10/SUM($M$10:$M$14)</f>
-        <v>0.8542735173981143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <f>M12+M14+M15</f>
+        <v>3706</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="5">
-        <v>101</v>
-      </c>
-      <c r="H11" s="5">
-        <v>982</v>
-      </c>
-      <c r="I11" s="4">
-        <f>SUM(G11:H11)</f>
-        <v>1083</v>
-      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="L11" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M11" s="10">
-        <v>3124</v>
+        <v>27816</v>
       </c>
       <c r="N11" s="8">
-        <f>M11/SUM($M$10:$M$14)</f>
-        <v>9.5942999293633494E-2</v>
+        <f>M11/SUM($M$11:$M$15)</f>
+        <v>0.8542735173981143</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.25">
@@ -4975,56 +4955,61 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G12" s="5">
-        <v>315</v>
+        <v>101</v>
       </c>
       <c r="H12" s="5">
-        <v>5826</v>
+        <v>982</v>
       </c>
       <c r="I12" s="4">
         <f>SUM(G12:H12)</f>
-        <v>6141</v>
+        <v>1083</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M12" s="10">
-        <v>1039</v>
+        <v>3124</v>
       </c>
       <c r="N12" s="8">
-        <f>M12/SUM($M$10:$M$14)</f>
-        <v>3.1909339393753261E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <f>M12/SUM($M$11:$M$15)</f>
+        <v>9.5942999293633494E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4">
-        <f>SUM(G11:G12)</f>
-        <v>416</v>
-      </c>
-      <c r="H13" s="4">
-        <f>SUM(H11:H12)</f>
-        <v>6808</v>
-      </c>
-      <c r="I13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="5">
+        <v>315</v>
+      </c>
+      <c r="H13" s="5">
+        <v>5826</v>
+      </c>
+      <c r="I13" s="4">
+        <f>SUM(G13:H13)</f>
+        <v>6141</v>
+      </c>
       <c r="L13" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M13" s="10">
-        <v>311</v>
+        <v>1039</v>
       </c>
       <c r="N13" s="8">
-        <f>M13/SUM($M$10:$M$14)</f>
-        <v>9.551303706888609E-3</v>
+        <f>M13/SUM($M$11:$M$15)</f>
+        <v>3.1909339393753261E-2</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -5033,89 +5018,99 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="4">
+        <f>SUM(G12:G13)</f>
+        <v>416</v>
+      </c>
+      <c r="H14" s="4">
+        <f>SUM(H12:H13)</f>
+        <v>6808</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="L14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="10">
+        <v>311</v>
+      </c>
+      <c r="N14" s="8">
+        <f>M14/SUM($M$11:$M$15)</f>
+        <v>9.551303706888609E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="L15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M15" s="10">
         <v>271</v>
       </c>
-      <c r="N14" s="8">
-        <f>M14/SUM($M$10:$M$14)</f>
+      <c r="N15" s="8">
+        <f>M15/SUM($M$11:$M$15)</f>
         <v>8.3228402076103315E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <f>G11/G7</f>
-        <v>6.1547836684948204E-2</v>
-      </c>
-      <c r="C15" s="4">
-        <f>H11/H7</f>
-        <v>0.11824202287778447</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="5">
-        <v>6.1499999999999999E-2</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0.1182</v>
-      </c>
-      <c r="I15" s="4">
-        <f>I11/I7</f>
-        <v>0.10888799517393927</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <f>G12/G8</f>
-        <v>0.17726505346088914</v>
+        <v>6.1547836684948204E-2</v>
       </c>
       <c r="C16" s="4">
         <f>H12/H8</f>
-        <v>0.31876128467472781</v>
+        <v>0.11824202287778447</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G16" s="5">
-        <v>0.17730000000000001</v>
+        <v>6.1499999999999999E-2</v>
       </c>
       <c r="H16" s="5">
-        <v>0.31879999999999997</v>
+        <v>0.1182</v>
       </c>
       <c r="I16" s="4">
         <f>I12/I8</f>
+        <v>0.10888799517393927</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <f>G13/G9</f>
+        <v>0.17726505346088914</v>
+      </c>
+      <c r="C17" s="4">
+        <f>H13/H9</f>
+        <v>0.31876128467472781</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.17730000000000001</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I17" s="4">
+        <f>I13/I9</f>
         <v>0.30622319736710879</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4">
-        <f>G13/G9</f>
-        <v>0.12170860152135751</v>
-      </c>
-      <c r="H17" s="4">
-        <f>H13/H9</f>
-        <v>0.25611315928071626</v>
-      </c>
-      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
@@ -5123,125 +5118,131 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="G18" s="4">
+        <f>G14/G10</f>
+        <v>0.12170860152135751</v>
+      </c>
+      <c r="H18" s="4">
+        <f>H14/H10</f>
+        <v>0.25611315928071626</v>
+      </c>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4">
-        <f>$H$16/G15</f>
-        <v>5.1837398373983739</v>
-      </c>
-      <c r="H19" s="4">
-        <f>$H$16/H15</f>
-        <v>2.6971235194585446</v>
-      </c>
-      <c r="I19" s="4">
-        <f>I16/I15</f>
-        <v>2.8122769353769752</v>
-      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4">
-        <f>$H$16/G16</f>
-        <v>1.7980823463056963</v>
+        <f>$H$17/G16</f>
+        <v>5.1837398373983739</v>
       </c>
       <c r="H20" s="4">
-        <f>$H$16/H16</f>
-        <v>1</v>
-      </c>
-      <c r="I20" s="4"/>
+        <f>$H$17/H16</f>
+        <v>2.6971235194585446</v>
+      </c>
+      <c r="I20" s="4">
+        <f>I17/I16</f>
+        <v>2.8122769353769752</v>
+      </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <v>619.58789999999999</v>
-      </c>
-      <c r="C21">
-        <v>2444.5385999999999</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4">
+        <f>$H$17/G17</f>
+        <v>1.7980823463056963</v>
+      </c>
       <c r="H21" s="4">
-        <f>H17/G17</f>
-        <v>2.1043143712055006</v>
+        <f>$H$17/H17</f>
+        <v>1</v>
       </c>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>369.09059999999999</v>
+        <v>619.58789999999999</v>
+      </c>
+      <c r="C22">
+        <v>2444.5385999999999</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="H22" s="4">
+        <f>H18/G18</f>
+        <v>2.1043143712055006</v>
+      </c>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="4">
-        <v>422.55772357723578</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1666.5752961082908</v>
+      <c r="B23">
+        <v>369.09059999999999</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4">
-        <f>($H$16*G7 - G11)/(1 - $H$16)</f>
-        <v>619.71638285378742</v>
-      </c>
-      <c r="H23" s="4">
-        <f>($H$16*H7-H11)/(1-$H$16)</f>
-        <v>2445.1467997651198</v>
-      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="4">
-        <v>251.39593908629433</v>
+        <v>422.55772357723578</v>
       </c>
       <c r="C24" s="4">
-        <v>0</v>
+        <v>1666.5752961082908</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4">
-        <f>($H$16*G8-G12)/(1-$H$16)</f>
-        <v>369.21256605989419</v>
+        <f>($H$17*G8 - G12)/(1 - $H$17)</f>
+        <v>619.71638285378742</v>
       </c>
       <c r="H24" s="4">
-        <f>($H$16*H8-H12)/(1-$H$16)</f>
-        <v>1.0387551379913817</v>
+        <f>($H$17*H8-H12)/(1-$H$17)</f>
+        <v>2445.1467997651198</v>
       </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="4">
+        <v>251.39593908629433</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="G25" s="4">
+        <f>($H$17*G9-G13)/(1-$H$17)</f>
+        <v>369.21256605989419</v>
+      </c>
+      <c r="H25" s="4">
+        <f>($H$17*H9-H13)/(1-$H$17)</f>
+        <v>1.0387551379913817</v>
+      </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
@@ -5258,40 +5259,31 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4">
-        <f>G7+G23</f>
-        <v>2260.7163828537873</v>
-      </c>
-      <c r="H27" s="4">
-        <f>H7+H23</f>
-        <v>10750.14679976512</v>
-      </c>
-      <c r="I27" s="4">
-        <f>SUM(G27:H27)</f>
-        <v>13010.863182618907</v>
-      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4">
         <f>G8+G24</f>
-        <v>2146.212566059894</v>
+        <v>2260.7163828537873</v>
       </c>
       <c r="H28" s="4">
         <f>H8+H24</f>
-        <v>18278.03875513799</v>
+        <v>10750.14679976512</v>
       </c>
       <c r="I28" s="4">
         <f>SUM(G28:H28)</f>
-        <v>20424.251321197884</v>
+        <v>13010.863182618907</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
@@ -5301,14 +5293,17 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4">
-        <f>SUM(G27:G28)</f>
-        <v>4406.9289489136809</v>
+        <f>G9+G25</f>
+        <v>2146.212566059894</v>
       </c>
       <c r="H29" s="4">
-        <f>SUM(H27:H28)</f>
-        <v>29028.18555490311</v>
-      </c>
-      <c r="I29" s="4"/>
+        <f>H9+H25</f>
+        <v>18278.03875513799</v>
+      </c>
+      <c r="I29" s="4">
+        <f>SUM(G29:H29)</f>
+        <v>20424.251321197884</v>
+      </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
@@ -5316,79 +5311,79 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="G30" s="4">
+        <f>SUM(G28:G29)</f>
+        <v>4406.9289489136809</v>
+      </c>
+      <c r="H30" s="4">
+        <f>SUM(H28:H29)</f>
+        <v>29028.18555490311</v>
+      </c>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="4">
-        <f>G19*G11</f>
-        <v>523.55772357723572</v>
-      </c>
-      <c r="C31" s="4">
-        <f>H19*H11</f>
-        <v>2648.5752961082908</v>
-      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="4">
-        <f>G23+G11</f>
-        <v>720.71638285378742</v>
-      </c>
-      <c r="H31" s="4">
-        <f>H23+H11</f>
-        <v>3427.1467997651198</v>
-      </c>
-      <c r="I31" s="4">
-        <f>SUM(G31:H31)</f>
-        <v>4147.8631826189076</v>
-      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="4">
         <f>G20*G12</f>
-        <v>566.39593908629433</v>
+        <v>523.55772357723572</v>
       </c>
       <c r="C32" s="4">
         <f>H20*H12</f>
-        <v>5826</v>
+        <v>2648.5752961082908</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4">
         <f>G24+G12</f>
-        <v>684.21256605989424</v>
+        <v>720.71638285378742</v>
       </c>
       <c r="H32" s="4">
         <f>H24+H12</f>
-        <v>5827.0387551379918</v>
+        <v>3427.1467997651198</v>
       </c>
       <c r="I32" s="4">
         <f>SUM(G32:H32)</f>
-        <v>6511.2513211978858</v>
+        <v>4147.8631826189076</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="4">
+        <f>G21*G13</f>
+        <v>566.39593908629433</v>
+      </c>
+      <c r="C33" s="4">
+        <f>H21*H13</f>
+        <v>5826</v>
+      </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4">
-        <f>SUM(G31:G32)</f>
-        <v>1404.9289489136818</v>
+        <f>G25+G13</f>
+        <v>684.21256605989424</v>
       </c>
       <c r="H33" s="4">
-        <f>SUM(H31:H32)</f>
-        <v>9254.1855549031116</v>
-      </c>
-      <c r="I33" s="4"/>
+        <f>H25+H13</f>
+        <v>5827.0387551379918</v>
+      </c>
+      <c r="I33" s="4">
+        <f>SUM(G33:H33)</f>
+        <v>6511.2513211978858</v>
+      </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
@@ -5396,46 +5391,41 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="G34" s="4">
+        <f>SUM(G32:G33)</f>
+        <v>1404.9289489136818</v>
+      </c>
+      <c r="H34" s="4">
+        <f>SUM(H32:H33)</f>
+        <v>9254.1855549031116</v>
+      </c>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4">
-        <f t="shared" ref="G35:I36" si="0">G31/G27</f>
-        <v>0.31880000000000003</v>
-      </c>
-      <c r="H35" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31879999999999997</v>
-      </c>
-      <c r="I35" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
-      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G36:I37" si="0">G32/G28</f>
         <v>0.31880000000000003</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
+        <v>0.31879999999999997</v>
       </c>
       <c r="I36" s="4">
         <f t="shared" si="0"/>
@@ -5446,151 +5436,172 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4">
-        <f>G33/G29</f>
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="I37" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4">
+        <f>G34/G30</f>
         <v>0.31880000000000008</v>
       </c>
-      <c r="H37" s="4">
-        <f>H33/H29</f>
+      <c r="H38" s="4">
+        <f>H34/H30</f>
         <v>0.31880000000000003</v>
       </c>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="41" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
-      <c r="C41" s="6" t="s">
+      <c r="I38" s="4"/>
+    </row>
+    <row r="42" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="5">
-        <v>750</v>
-      </c>
-      <c r="D42" s="5">
-        <v>1238</v>
       </c>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="5">
+        <v>750</v>
+      </c>
+      <c r="D43" s="5">
+        <v>1238</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>75</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D44" s="5">
         <v>498</v>
       </c>
-      <c r="E43" s="4">
-        <f>SUM(C42:D43)</f>
+      <c r="E44" s="4">
+        <f>SUM(C43:D44)</f>
         <v>2561</v>
       </c>
-      <c r="F43">
-        <f>D43/C43</f>
+      <c r="F44">
+        <f>D44/C44</f>
         <v>6.64</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4">
-        <f>C43/C42</f>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4">
+        <f>C44/C43</f>
         <v>0.1</v>
       </c>
-      <c r="D44" s="4">
-        <f>D43/D42</f>
+      <c r="D45" s="4">
+        <f>D44/D43</f>
         <v>0.40226171243941844</v>
       </c>
-      <c r="E44" s="4">
-        <f>D44/C44</f>
+      <c r="E45" s="4">
+        <f>D45/C45</f>
         <v>4.0226171243941842</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
-      <c r="C45" s="6" t="s">
+    <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="5">
-        <v>267</v>
-      </c>
-      <c r="D46" s="5">
-        <v>1721</v>
       </c>
       <c r="E46" s="4"/>
     </row>
     <row r="47" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="5">
+        <v>267</v>
+      </c>
+      <c r="D47" s="5">
+        <v>1721</v>
+      </c>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>21</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D48" s="5">
         <v>552</v>
       </c>
-      <c r="E47" s="4">
-        <f>SUM(C46:D47)</f>
+      <c r="E48" s="4">
+        <f>SUM(C47:D48)</f>
         <v>2561</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="2:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="B50" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="5">
-        <v>881</v>
-      </c>
-      <c r="D50" s="5">
-        <v>1107</v>
       </c>
       <c r="E50" s="4"/>
     </row>
     <row r="51" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="5">
+        <v>881</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1107</v>
+      </c>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>90</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D52" s="5">
         <v>483</v>
       </c>
-      <c r="E51" s="4">
-        <f>SUM(C50:D51)</f>
+      <c r="E52" s="4">
+        <f>SUM(C51:D52)</f>
         <v>2561</v>
       </c>
     </row>
@@ -5601,6 +5612,7 @@
     <hyperlink ref="B3" r:id="rId3" xr:uid="{B88AF874-80B7-F843-B08B-3A0D063425A5}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{A5515785-4094-994E-9541-747616D5BC0D}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{62FEC5B1-56D8-7740-8ED0-F73ED66D809E}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{453584B6-2853-C447-90CD-97D59EEC4005}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5613,7 +5625,7 @@
   </sheetPr>
   <dimension ref="B1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create Data class and add pie charts
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Code/debias-ml/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Project/Code/debias-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD400838-AD8D-3F49-B025-6D8DBFFD8C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8F1137-116E-F34C-851F-70690BE296E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="7240" windowWidth="26180" windowHeight="13760" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="3320" yWindow="740" windowWidth="46480" windowHeight="30500" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="60">
   <si>
     <t>Training time</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>Bias Factors</t>
-  </si>
-  <si>
-    <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=8YJwqUhK1jSHPi6TkpQ9</t>
   </si>
   <si>
     <t>Bias</t>
@@ -2530,7 +2527,7 @@
   <dimension ref="B2:M134"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C20"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2775,6 +2772,10 @@
       <c r="F9" s="2">
         <v>65.601459000000006</v>
       </c>
+      <c r="G9" s="4">
+        <f>34/30</f>
+        <v>1.1333333333333333</v>
+      </c>
       <c r="I9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2807,6 +2808,10 @@
       <c r="F10" s="2">
         <v>4.8730000000000002E-2</v>
       </c>
+      <c r="G10" s="4">
+        <f>2+165*(1/20+128/30000)</f>
+        <v>10.954000000000001</v>
+      </c>
       <c r="I10" s="4" t="s">
         <v>13</v>
       </c>
@@ -2838,6 +2843,10 @@
       </c>
       <c r="F11" s="2">
         <v>0.71519900000000003</v>
+      </c>
+      <c r="G11" s="4">
+        <f>G10/G9</f>
+        <v>9.6652941176470595</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>15</v>
@@ -4781,10 +4790,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D1:D1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4811,15 +4820,15 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
-        <v>43503</v>
+        <v>43506</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
-        <v>43506</v>
+        <v>43507</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>58</v>
@@ -4827,87 +4836,99 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
-        <v>43507</v>
+        <v>43513</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="11">
-        <v>43513</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1641</v>
+      </c>
+      <c r="H7" s="5">
+        <v>8305</v>
+      </c>
+      <c r="I7" s="4">
+        <f>SUM(G7:H7)</f>
+        <v>9946</v>
+      </c>
+      <c r="N7">
+        <f>N8/(N8+N9)</f>
+        <v>0.88618285679186759</v>
+      </c>
+      <c r="O7">
+        <f>M10/SUM(M10:M15)</f>
+        <v>0.8542735173981143</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="B8" s="4">
+        <f>SUM(G7:H8)</f>
+        <v>30000</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="5">
-        <v>1641</v>
+        <v>1777</v>
       </c>
       <c r="H8" s="5">
-        <v>8305</v>
+        <v>18277</v>
       </c>
       <c r="I8" s="4">
         <f>SUM(G8:H8)</f>
-        <v>9946</v>
+        <v>20054</v>
       </c>
       <c r="N8">
-        <f>N9/(N9+N10)</f>
-        <v>0.88618285679186759</v>
-      </c>
-      <c r="O8">
-        <f>M11/SUM(M11:M16)</f>
-        <v>0.8542735173981143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
-        <f>SUM(G8:H9)</f>
-        <v>30000</v>
-      </c>
+        <f>M10+M12</f>
+        <v>28855</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1777</v>
-      </c>
-      <c r="H9" s="5">
-        <v>18277</v>
-      </c>
-      <c r="I9" s="4">
-        <f>SUM(G9:H9)</f>
-        <v>20054</v>
-      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4">
+        <f>SUM(G7:G8)</f>
+        <v>3418</v>
+      </c>
+      <c r="H9" s="4">
+        <f>SUM(H7:H8)</f>
+        <v>26582</v>
+      </c>
+      <c r="I9" s="4"/>
       <c r="N9">
-        <f>M11+M13</f>
-        <v>28855</v>
+        <f>M11+M13+M14</f>
+        <v>3706</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -4916,38 +4937,49 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4">
-        <f>SUM(G8:G9)</f>
-        <v>3418</v>
-      </c>
-      <c r="H10" s="4">
-        <f>SUM(H8:H9)</f>
-        <v>26582</v>
-      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="N10">
-        <f>M12+M14+M15</f>
-        <v>3706</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="10">
+        <v>27816</v>
+      </c>
+      <c r="N10" s="8">
+        <f>M10/SUM($M$10:$M$14)</f>
+        <v>0.8542735173981143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="5">
+        <v>101</v>
+      </c>
+      <c r="H11" s="5">
+        <v>982</v>
+      </c>
+      <c r="I11" s="4">
+        <f>SUM(G11:H11)</f>
+        <v>1083</v>
+      </c>
       <c r="L11" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M11" s="10">
-        <v>27816</v>
+        <v>3124</v>
       </c>
       <c r="N11" s="8">
-        <f>M11/SUM($M$11:$M$15)</f>
-        <v>0.8542735173981143</v>
+        <f>M11/SUM($M$10:$M$14)</f>
+        <v>9.5942999293633494E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.25">
@@ -4955,61 +4987,56 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="5">
-        <v>101</v>
+        <v>315</v>
       </c>
       <c r="H12" s="5">
-        <v>982</v>
+        <v>5826</v>
       </c>
       <c r="I12" s="4">
         <f>SUM(G12:H12)</f>
-        <v>1083</v>
+        <v>6141</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M12" s="10">
-        <v>3124</v>
+        <v>1039</v>
       </c>
       <c r="N12" s="8">
-        <f>M12/SUM($M$11:$M$15)</f>
-        <v>9.5942999293633494E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+        <f>M12/SUM($M$10:$M$14)</f>
+        <v>3.1909339393753261E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="5">
-        <v>315</v>
-      </c>
-      <c r="H13" s="5">
-        <v>5826</v>
-      </c>
-      <c r="I13" s="4">
-        <f>SUM(G13:H13)</f>
-        <v>6141</v>
-      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4">
+        <f>SUM(G11:G12)</f>
+        <v>416</v>
+      </c>
+      <c r="H13" s="4">
+        <f>SUM(H11:H12)</f>
+        <v>6808</v>
+      </c>
+      <c r="I13" s="4"/>
       <c r="L13" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M13" s="10">
-        <v>1039</v>
+        <v>311</v>
       </c>
       <c r="N13" s="8">
-        <f>M13/SUM($M$11:$M$15)</f>
-        <v>3.1909339393753261E-2</v>
+        <f>M13/SUM($M$10:$M$14)</f>
+        <v>9.551303706888609E-3</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -5018,99 +5045,89 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4">
-        <f>SUM(G12:G13)</f>
-        <v>416</v>
-      </c>
-      <c r="H14" s="4">
-        <f>SUM(H12:H13)</f>
-        <v>6808</v>
-      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="L14" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M14" s="10">
-        <v>311</v>
+        <v>271</v>
       </c>
       <c r="N14" s="8">
-        <f>M14/SUM($M$11:$M$15)</f>
-        <v>9.551303706888609E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+        <f>M14/SUM($M$10:$M$14)</f>
+        <v>8.3228402076103315E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <f>G11/G7</f>
+        <v>6.1547836684948204E-2</v>
+      </c>
+      <c r="C15" s="4">
+        <f>H11/H7</f>
+        <v>0.11824202287778447</v>
+      </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="L15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="10">
-        <v>271</v>
-      </c>
-      <c r="N15" s="8">
-        <f>M15/SUM($M$11:$M$15)</f>
-        <v>8.3228402076103315E-3</v>
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="5">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.1182</v>
+      </c>
+      <c r="I15" s="4">
+        <f>I11/I7</f>
+        <v>0.10888799517393927</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <f>G12/G8</f>
-        <v>6.1547836684948204E-2</v>
+        <v>0.17726505346088914</v>
       </c>
       <c r="C16" s="4">
         <f>H12/H8</f>
-        <v>0.11824202287778447</v>
+        <v>0.31876128467472781</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="5">
-        <v>6.1499999999999999E-2</v>
+        <v>0.17730000000000001</v>
       </c>
       <c r="H16" s="5">
-        <v>0.1182</v>
+        <v>0.31879999999999997</v>
       </c>
       <c r="I16" s="4">
         <f>I12/I8</f>
-        <v>0.10888799517393927</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
+        <v>0.30622319736710879</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4">
         <f>G13/G9</f>
-        <v>0.17726505346088914</v>
-      </c>
-      <c r="C17" s="4">
+        <v>0.12170860152135751</v>
+      </c>
+      <c r="H17" s="4">
         <f>H13/H9</f>
-        <v>0.31876128467472781</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0.17730000000000001</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0.31879999999999997</v>
-      </c>
-      <c r="I17" s="4">
-        <f>I13/I9</f>
-        <v>0.30622319736710879</v>
-      </c>
+        <v>0.25611315928071626</v>
+      </c>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
@@ -5118,131 +5135,125 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4">
-        <f>G14/G10</f>
-        <v>0.12170860152135751</v>
-      </c>
-      <c r="H18" s="4">
-        <f>H14/H10</f>
-        <v>0.25611315928071626</v>
-      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="G19" s="4">
+        <f>$H$16/G15</f>
+        <v>5.1837398373983739</v>
+      </c>
+      <c r="H19" s="4">
+        <f>$H$16/H15</f>
+        <v>2.6971235194585446</v>
+      </c>
+      <c r="I19" s="4">
+        <f>I16/I15</f>
+        <v>2.8122769353769752</v>
+      </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4">
-        <f>$H$17/G16</f>
-        <v>5.1837398373983739</v>
+        <f>$H$16/G16</f>
+        <v>1.7980823463056963</v>
       </c>
       <c r="H20" s="4">
-        <f>$H$17/H16</f>
-        <v>2.6971235194585446</v>
-      </c>
-      <c r="I20" s="4">
-        <f>I17/I16</f>
-        <v>2.8122769353769752</v>
-      </c>
+        <f>$H$16/H16</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="B21">
+        <v>619.58789999999999</v>
+      </c>
+      <c r="C21">
+        <v>2444.5385999999999</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4">
-        <f>$H$17/G17</f>
-        <v>1.7980823463056963</v>
-      </c>
+      <c r="G21" s="4"/>
       <c r="H21" s="4">
-        <f>$H$17/H17</f>
-        <v>1</v>
+        <f>H17/G17</f>
+        <v>2.1043143712055006</v>
       </c>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>619.58789999999999</v>
-      </c>
-      <c r="C22">
-        <v>2444.5385999999999</v>
+        <v>369.09059999999999</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4">
-        <f>H18/G18</f>
-        <v>2.1043143712055006</v>
-      </c>
+      <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <v>369.09059999999999</v>
+      <c r="B23" s="4">
+        <v>422.55772357723578</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1666.5752961082908</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="G23" s="4">
+        <f>($H$16*G7 - G11)/(1 - $H$16)</f>
+        <v>619.71638285378742</v>
+      </c>
+      <c r="H23" s="4">
+        <f>($H$16*H7-H11)/(1-$H$16)</f>
+        <v>2445.1467997651198</v>
+      </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="4">
-        <v>422.55772357723578</v>
+        <v>251.39593908629433</v>
       </c>
       <c r="C24" s="4">
-        <v>1666.5752961082908</v>
+        <v>0</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4">
-        <f>($H$17*G8 - G12)/(1 - $H$17)</f>
-        <v>619.71638285378742</v>
+        <f>($H$16*G8-G12)/(1-$H$16)</f>
+        <v>369.21256605989419</v>
       </c>
       <c r="H24" s="4">
-        <f>($H$17*H8-H12)/(1-$H$17)</f>
-        <v>2445.1467997651198</v>
+        <f>($H$16*H8-H12)/(1-$H$16)</f>
+        <v>1.0387551379913817</v>
       </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="4">
-        <v>251.39593908629433</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0</v>
-      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="4">
-        <f>($H$17*G9-G13)/(1-$H$17)</f>
-        <v>369.21256605989419</v>
-      </c>
-      <c r="H25" s="4">
-        <f>($H$17*H9-H13)/(1-$H$17)</f>
-        <v>1.0387551379913817</v>
-      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
@@ -5259,31 +5270,40 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="G27" s="4">
+        <f>G7+G23</f>
+        <v>2260.7163828537873</v>
+      </c>
+      <c r="H27" s="4">
+        <f>H7+H23</f>
+        <v>10750.14679976512</v>
+      </c>
+      <c r="I27" s="4">
+        <f>SUM(G27:H27)</f>
+        <v>13010.863182618907</v>
+      </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4">
         <f>G8+G24</f>
-        <v>2260.7163828537873</v>
+        <v>2146.212566059894</v>
       </c>
       <c r="H28" s="4">
         <f>H8+H24</f>
-        <v>10750.14679976512</v>
+        <v>18278.03875513799</v>
       </c>
       <c r="I28" s="4">
         <f>SUM(G28:H28)</f>
-        <v>13010.863182618907</v>
+        <v>20424.251321197884</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
@@ -5293,17 +5313,14 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4">
-        <f>G9+G25</f>
-        <v>2146.212566059894</v>
+        <f>SUM(G27:G28)</f>
+        <v>4406.9289489136809</v>
       </c>
       <c r="H29" s="4">
-        <f>H9+H25</f>
-        <v>18278.03875513799</v>
-      </c>
-      <c r="I29" s="4">
-        <f>SUM(G29:H29)</f>
-        <v>20424.251321197884</v>
-      </c>
+        <f>SUM(H27:H28)</f>
+        <v>29028.18555490311</v>
+      </c>
+      <c r="I29" s="4"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
@@ -5311,79 +5328,79 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4">
-        <f>SUM(G28:G29)</f>
-        <v>4406.9289489136809</v>
-      </c>
-      <c r="H30" s="4">
-        <f>SUM(H28:H29)</f>
-        <v>29028.18555490311</v>
-      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="4">
+        <f>G19*G11</f>
+        <v>523.55772357723572</v>
+      </c>
+      <c r="C31" s="4">
+        <f>H19*H11</f>
+        <v>2648.5752961082908</v>
+      </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
+      <c r="G31" s="4">
+        <f>G23+G11</f>
+        <v>720.71638285378742</v>
+      </c>
+      <c r="H31" s="4">
+        <f>H23+H11</f>
+        <v>3427.1467997651198</v>
+      </c>
+      <c r="I31" s="4">
+        <f>SUM(G31:H31)</f>
+        <v>4147.8631826189076</v>
+      </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="4">
         <f>G20*G12</f>
-        <v>523.55772357723572</v>
+        <v>566.39593908629433</v>
       </c>
       <c r="C32" s="4">
         <f>H20*H12</f>
-        <v>2648.5752961082908</v>
+        <v>5826</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4">
         <f>G24+G12</f>
-        <v>720.71638285378742</v>
+        <v>684.21256605989424</v>
       </c>
       <c r="H32" s="4">
         <f>H24+H12</f>
-        <v>3427.1467997651198</v>
+        <v>5827.0387551379918</v>
       </c>
       <c r="I32" s="4">
         <f>SUM(G32:H32)</f>
-        <v>4147.8631826189076</v>
+        <v>6511.2513211978858</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="4">
-        <f>G21*G13</f>
-        <v>566.39593908629433</v>
-      </c>
-      <c r="C33" s="4">
-        <f>H21*H13</f>
-        <v>5826</v>
-      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4">
-        <f>G25+G13</f>
-        <v>684.21256605989424</v>
+        <f>SUM(G31:G32)</f>
+        <v>1404.9289489136818</v>
       </c>
       <c r="H33" s="4">
-        <f>H25+H13</f>
-        <v>5827.0387551379918</v>
-      </c>
-      <c r="I33" s="4">
-        <f>SUM(G33:H33)</f>
-        <v>6511.2513211978858</v>
-      </c>
+        <f>SUM(H31:H32)</f>
+        <v>9254.1855549031116</v>
+      </c>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
@@ -5391,41 +5408,46 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4">
-        <f>SUM(G32:G33)</f>
-        <v>1404.9289489136818</v>
-      </c>
-      <c r="H34" s="4">
-        <f>SUM(H32:H33)</f>
-        <v>9254.1855549031116</v>
-      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
+      <c r="G35" s="4">
+        <f t="shared" ref="G35:I36" si="0">G31/G27</f>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I35" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4">
-        <f t="shared" ref="G36:I37" si="0">G32/G28</f>
+        <f t="shared" si="0"/>
         <v>0.31880000000000003</v>
       </c>
       <c r="H36" s="4">
         <f t="shared" si="0"/>
-        <v>0.31879999999999997</v>
+        <v>0.31880000000000003</v>
       </c>
       <c r="I36" s="4">
         <f t="shared" si="0"/>
@@ -5436,172 +5458,151 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4">
-        <f t="shared" si="0"/>
+        <f>G33/G29</f>
+        <v>0.31880000000000008</v>
+      </c>
+      <c r="H37" s="4">
+        <f>H33/H29</f>
         <v>0.31880000000000003</v>
       </c>
-      <c r="H37" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
-      </c>
-      <c r="I37" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4">
-        <f>G34/G30</f>
-        <v>0.31880000000000008</v>
-      </c>
-      <c r="H38" s="4">
-        <f>H34/H30</f>
-        <v>0.31880000000000003</v>
-      </c>
-      <c r="I38" s="4"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="41" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
-      <c r="C42" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>24</v>
+      <c r="B42" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="5">
+        <v>750</v>
+      </c>
+      <c r="D42" s="5">
+        <v>1238</v>
       </c>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="5">
+        <v>75</v>
+      </c>
+      <c r="D43" s="5">
+        <v>498</v>
+      </c>
+      <c r="E43" s="4">
+        <f>SUM(C42:D43)</f>
+        <v>2561</v>
+      </c>
+      <c r="F43">
+        <f>D43/C43</f>
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4">
+        <f>C43/C42</f>
+        <v>0.1</v>
+      </c>
+      <c r="D44" s="4">
+        <f>D43/D42</f>
+        <v>0.40226171243941844</v>
+      </c>
+      <c r="E44" s="4">
+        <f>D44/C44</f>
+        <v>4.0226171243941842</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="5">
-        <v>750</v>
-      </c>
-      <c r="D43" s="5">
-        <v>1238</v>
-      </c>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C44" s="5">
-        <v>75</v>
-      </c>
-      <c r="D44" s="5">
-        <v>498</v>
-      </c>
-      <c r="E44" s="4">
-        <f>SUM(C43:D44)</f>
-        <v>2561</v>
-      </c>
-      <c r="F44">
-        <f>D44/C44</f>
-        <v>6.64</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="4"/>
-      <c r="C45" s="4">
-        <f>C44/C43</f>
-        <v>0.1</v>
-      </c>
-      <c r="D45" s="4">
-        <f>D44/D43</f>
-        <v>0.40226171243941844</v>
-      </c>
-      <c r="E45" s="4">
-        <f>D45/C45</f>
-        <v>4.0226171243941842</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
-      <c r="C46" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>32</v>
+      <c r="C46" s="5">
+        <v>267</v>
+      </c>
+      <c r="D46" s="5">
+        <v>1721</v>
       </c>
       <c r="E46" s="4"/>
     </row>
     <row r="47" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="5">
+        <v>21</v>
+      </c>
+      <c r="D47" s="5">
+        <v>552</v>
+      </c>
+      <c r="E47" s="4">
+        <f>SUM(C46:D47)</f>
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="5">
-        <v>267</v>
-      </c>
-      <c r="D47" s="5">
-        <v>1721</v>
-      </c>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B48" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C48" s="5">
-        <v>21</v>
-      </c>
-      <c r="D48" s="5">
-        <v>552</v>
-      </c>
-      <c r="E48" s="4">
-        <f>SUM(C47:D48)</f>
-        <v>2561</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="2:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
-      <c r="C50" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>36</v>
+      <c r="C50" s="5">
+        <v>881</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1107</v>
       </c>
       <c r="E50" s="4"/>
     </row>
     <row r="51" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C51" s="5">
-        <v>881</v>
+        <v>90</v>
       </c>
       <c r="D51" s="5">
-        <v>1107</v>
-      </c>
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="2:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="B52" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" s="5">
-        <v>90</v>
-      </c>
-      <c r="D52" s="5">
         <v>483</v>
       </c>
-      <c r="E52" s="4">
-        <f>SUM(C51:D52)</f>
+      <c r="E51" s="4">
+        <f>SUM(C50:D51)</f>
         <v>2561</v>
       </c>
     </row>
@@ -5609,10 +5610,9 @@
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{9C39114D-177D-874F-9648-8D0623AF7627}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{62BC5D29-BC2E-BE4F-9971-6E1802D9851C}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{B88AF874-80B7-F843-B08B-3A0D063425A5}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{A5515785-4094-994E-9541-747616D5BC0D}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{62FEC5B1-56D8-7740-8ED0-F73ED66D809E}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{453584B6-2853-C447-90CD-97D59EEC4005}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{A5515785-4094-994E-9541-747616D5BC0D}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{62FEC5B1-56D8-7740-8ED0-F73ED66D809E}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{453584B6-2853-C447-90CD-97D59EEC4005}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5642,7 +5642,7 @@
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
       <c r="D2" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="16"/>
       <c r="F2" s="22" t="s">
@@ -5657,7 +5657,7 @@
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
       <c r="D3" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="28">
@@ -5672,7 +5672,7 @@
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Split report into three parts
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Project/Code/debias-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8F1137-116E-F34C-851F-70690BE296E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6359051D-E166-724B-9001-A97F9932C574}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="740" windowWidth="46480" windowHeight="30500" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="38180" yWindow="5320" windowWidth="34960" windowHeight="23880" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
   <si>
     <t>Training time</t>
   </si>
@@ -212,6 +212,24 @@
   </si>
   <si>
     <t>http://share.streamlit.io/0.25.0-cdyb/index.html?id=2vHQ1bySr6a1FnzM6x14De</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.35.0-2Ln8d/index.html?id=UnGJdUneC6GrkBauP1N7s8</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.35.0-2Ln8d/index.html?id=LFgZszBLUBjrGzRVMfxJTm</t>
+  </si>
+  <si>
+    <t>data analysis</t>
+  </si>
+  <si>
+    <t>model analysis</t>
+  </si>
+  <si>
+    <t>oversampling analysis</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.35.0-2Ln8d/index.html?id=6emvf2pnq1BsSSNkZB6iVA</t>
   </si>
 </sst>
 </file>
@@ -397,9 +415,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -440,6 +455,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4790,227 +4808,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="11">
+      <c r="B1" s="10">
         <v>43501</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+      <c r="B2" s="10">
         <v>43502</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
+      <c r="B3" s="10">
         <v>43506</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
+      <c r="B4" s="10">
         <v>43507</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
+      <c r="B5" s="10">
         <v>43513</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="230" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1641</v>
-      </c>
-      <c r="H7" s="5">
-        <v>8305</v>
-      </c>
-      <c r="I7" s="4">
-        <f>SUM(G7:H7)</f>
-        <v>9946</v>
-      </c>
-      <c r="N7">
-        <f>N8/(N8+N9)</f>
-        <v>0.88618285679186759</v>
-      </c>
-      <c r="O7">
-        <f>M10/SUM(M10:M15)</f>
-        <v>0.8542735173981143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <f>SUM(G7:H8)</f>
-        <v>30000</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1777</v>
-      </c>
-      <c r="H8" s="5">
-        <v>18277</v>
-      </c>
-      <c r="I8" s="4">
-        <f>SUM(G8:H8)</f>
-        <v>20054</v>
-      </c>
-      <c r="N8">
-        <f>M10+M12</f>
-        <v>28855</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="10">
+        <v>43588</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="10">
+        <v>43588</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="10">
+        <v>43588</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4">
-        <f>SUM(G7:G8)</f>
-        <v>3418</v>
-      </c>
-      <c r="H9" s="4">
-        <f>SUM(H7:H8)</f>
-        <v>26582</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="N9">
-        <f>M11+M13+M14</f>
-        <v>3706</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="L10" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="10">
-        <v>27816</v>
-      </c>
-      <c r="N10" s="8">
-        <f>M10/SUM($M$10:$M$14)</f>
+      <c r="G9" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1641</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8305</v>
+      </c>
+      <c r="I10" s="4">
+        <f>SUM(G10:H10)</f>
+        <v>9946</v>
+      </c>
+      <c r="N10">
+        <f>N11/(N11+N12)</f>
+        <v>0.88618285679186759</v>
+      </c>
+      <c r="O10">
+        <f>M13/SUM(M13:M18)</f>
         <v>0.8542735173981143</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
+      <c r="B11" s="4">
+        <f>SUM(G10:H11)</f>
+        <v>30000</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="5">
-        <v>101</v>
+        <v>1777</v>
       </c>
       <c r="H11" s="5">
-        <v>982</v>
+        <v>18277</v>
       </c>
       <c r="I11" s="4">
         <f>SUM(G11:H11)</f>
-        <v>1083</v>
-      </c>
-      <c r="L11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" s="10">
-        <v>3124</v>
-      </c>
-      <c r="N11" s="8">
-        <f>M11/SUM($M$10:$M$14)</f>
-        <v>9.5942999293633494E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.25">
+        <v>20054</v>
+      </c>
+      <c r="N11">
+        <f>M13+M15</f>
+        <v>28855</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="5">
-        <v>315</v>
-      </c>
-      <c r="H12" s="5">
-        <v>5826</v>
-      </c>
-      <c r="I12" s="4">
-        <f>SUM(G12:H12)</f>
-        <v>6141</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="10">
-        <v>1039</v>
-      </c>
-      <c r="N12" s="8">
-        <f>M12/SUM($M$10:$M$14)</f>
-        <v>3.1909339393753261E-2</v>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4">
+        <f>SUM(G10:G11)</f>
+        <v>3418</v>
+      </c>
+      <c r="H12" s="4">
+        <f>SUM(H10:H11)</f>
+        <v>26582</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="N12">
+        <f>M14+M16+M17</f>
+        <v>3706</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -5019,236 +4984,266 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4">
-        <f>SUM(G11:G12)</f>
-        <v>416</v>
-      </c>
-      <c r="H13" s="4">
-        <f>SUM(H11:H12)</f>
-        <v>6808</v>
-      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="L13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="10">
-        <v>311</v>
-      </c>
-      <c r="N13" s="8">
-        <f>M13/SUM($M$10:$M$14)</f>
-        <v>9.551303706888609E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="9">
+        <v>27816</v>
+      </c>
+      <c r="N13" s="7">
+        <f>M13/SUM($M$13:$M$17)</f>
+        <v>0.8542735173981143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="L14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="10">
-        <v>271</v>
-      </c>
-      <c r="N14" s="8">
-        <f>M14/SUM($M$10:$M$14)</f>
-        <v>8.3228402076103315E-3</v>
+      <c r="E14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="5">
+        <v>101</v>
+      </c>
+      <c r="H14" s="5">
+        <v>982</v>
+      </c>
+      <c r="I14" s="4">
+        <f>SUM(G14:H14)</f>
+        <v>1083</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="9">
+        <v>3124</v>
+      </c>
+      <c r="N14" s="7">
+        <f>M14/SUM($M$13:$M$17)</f>
+        <v>9.5942999293633494E-2</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <f>G11/G7</f>
-        <v>6.1547836684948204E-2</v>
-      </c>
-      <c r="C15" s="4">
-        <f>H11/H7</f>
-        <v>0.11824202287778447</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" s="5">
-        <v>6.1499999999999999E-2</v>
+        <v>315</v>
       </c>
       <c r="H15" s="5">
-        <v>0.1182</v>
+        <v>5826</v>
       </c>
       <c r="I15" s="4">
-        <f>I11/I7</f>
-        <v>0.10888799517393927</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <f>G12/G8</f>
-        <v>0.17726505346088914</v>
-      </c>
-      <c r="C16" s="4">
-        <f>H12/H8</f>
-        <v>0.31876128467472781</v>
-      </c>
+        <f>SUM(G15:H15)</f>
+        <v>6141</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="9">
+        <v>1039</v>
+      </c>
+      <c r="N15" s="7">
+        <f>M15/SUM($M$13:$M$17)</f>
+        <v>3.1909339393753261E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="5">
-        <v>0.17730000000000001</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0.31879999999999997</v>
-      </c>
-      <c r="I16" s="4">
-        <f>I12/I8</f>
-        <v>0.30622319736710879</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4">
+        <f>SUM(G14:G15)</f>
+        <v>416</v>
+      </c>
+      <c r="H16" s="4">
+        <f>SUM(H14:H15)</f>
+        <v>6808</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="L16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="9">
+        <v>311</v>
+      </c>
+      <c r="N16" s="7">
+        <f>M16/SUM($M$13:$M$17)</f>
+        <v>9.551303706888609E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4">
-        <f>G13/G9</f>
-        <v>0.12170860152135751</v>
-      </c>
-      <c r="H17" s="4">
-        <f>H13/H9</f>
-        <v>0.25611315928071626</v>
-      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
+      <c r="L17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="9">
+        <v>271</v>
+      </c>
+      <c r="N17" s="7">
+        <f>M17/SUM($M$13:$M$17)</f>
+        <v>8.3228402076103315E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="17" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <f>G14/G10</f>
+        <v>6.1547836684948204E-2</v>
+      </c>
+      <c r="C18" s="4">
+        <f>H14/H10</f>
+        <v>0.11824202287778447</v>
+      </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="5">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.1182</v>
+      </c>
+      <c r="I18" s="4">
+        <f>I14/I10</f>
+        <v>0.10888799517393927</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="17" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <f>G15/G11</f>
+        <v>0.17726505346088914</v>
+      </c>
+      <c r="C19" s="4">
+        <f>H15/H11</f>
+        <v>0.31876128467472781</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4">
-        <f>$H$16/G15</f>
-        <v>5.1837398373983739</v>
-      </c>
-      <c r="H19" s="4">
-        <f>$H$16/H15</f>
-        <v>2.6971235194585446</v>
+        <v>18</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.17730000000000001</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.31879999999999997</v>
       </c>
       <c r="I19" s="4">
-        <f>I16/I15</f>
-        <v>2.8122769353769752</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+        <f>I15/I11</f>
+        <v>0.30622319736710879</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4">
-        <f>$H$16/G16</f>
-        <v>1.7980823463056963</v>
+        <f>G16/G12</f>
+        <v>0.12170860152135751</v>
       </c>
       <c r="H20" s="4">
-        <f>$H$16/H16</f>
-        <v>1</v>
+        <f>H16/H12</f>
+        <v>0.25611315928071626</v>
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <v>619.58789999999999</v>
-      </c>
-      <c r="C21">
-        <v>2444.5385999999999</v>
-      </c>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4">
-        <f>H17/G17</f>
-        <v>2.1043143712055006</v>
-      </c>
+      <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <v>369.09059999999999</v>
-      </c>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="4">
-        <v>422.55772357723578</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1666.5752961082908</v>
-      </c>
+      <c r="G22" s="4">
+        <f>$H$19/G18</f>
+        <v>5.1837398373983739</v>
+      </c>
+      <c r="H22" s="4">
+        <f>$H$19/H18</f>
+        <v>2.6971235194585446</v>
+      </c>
+      <c r="I22" s="4">
+        <f>I19/I18</f>
+        <v>2.8122769353769752</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4">
-        <f>($H$16*G7 - G11)/(1 - $H$16)</f>
-        <v>619.71638285378742</v>
+        <f>$H$19/G19</f>
+        <v>1.7980823463056963</v>
       </c>
       <c r="H23" s="4">
-        <f>($H$16*H7-H11)/(1-$H$16)</f>
-        <v>2445.1467997651198</v>
+        <f>$H$19/H19</f>
+        <v>1</v>
       </c>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="4">
-        <v>251.39593908629433</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0</v>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>619.58789999999999</v>
+      </c>
+      <c r="C24">
+        <v>2444.5385999999999</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4">
-        <f>($H$16*G8-G12)/(1-$H$16)</f>
-        <v>369.21256605989419</v>
-      </c>
+      <c r="G24" s="4"/>
       <c r="H24" s="4">
-        <f>($H$16*H8-H12)/(1-$H$16)</f>
-        <v>1.0387551379913817</v>
+        <f>H20/G20</f>
+        <v>2.1043143712055006</v>
       </c>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>369.09059999999999</v>
+      </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -5256,135 +5251,123 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B26" s="4">
+        <v>422.55772357723578</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1666.5752961082908</v>
+      </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="G26" s="4">
+        <f>($H$19*G10 - G14)/(1 - $H$19)</f>
+        <v>619.71638285378742</v>
+      </c>
+      <c r="H26" s="4">
+        <f>($H$19*H10-H14)/(1-$H$19)</f>
+        <v>2445.1467997651198</v>
+      </c>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B27" s="4">
+        <v>251.39593908629433</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4">
-        <f>G7+G23</f>
-        <v>2260.7163828537873</v>
+        <f>($H$19*G11-G15)/(1-$H$19)</f>
+        <v>369.21256605989419</v>
       </c>
       <c r="H27" s="4">
-        <f>H7+H23</f>
-        <v>10750.14679976512</v>
-      </c>
-      <c r="I27" s="4">
-        <f>SUM(G27:H27)</f>
-        <v>13010.863182618907</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+        <f>($H$19*H11-H15)/(1-$H$19)</f>
+        <v>1.0387551379913817</v>
+      </c>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4">
-        <f>G8+G24</f>
-        <v>2146.212566059894</v>
-      </c>
-      <c r="H28" s="4">
-        <f>H8+H24</f>
-        <v>18278.03875513799</v>
-      </c>
-      <c r="I28" s="4">
-        <f>SUM(G28:H28)</f>
-        <v>20424.251321197884</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="4">
-        <f>SUM(G27:G28)</f>
-        <v>4406.9289489136809</v>
-      </c>
-      <c r="H29" s="4">
-        <f>SUM(H27:H28)</f>
-        <v>29028.18555490311</v>
-      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="4">
-        <f>G19*G11</f>
-        <v>523.55772357723572</v>
-      </c>
-      <c r="C31" s="4">
-        <f>H19*H11</f>
-        <v>2648.5752961082908</v>
-      </c>
+      <c r="G30" s="4">
+        <f>G10+G26</f>
+        <v>2260.7163828537873</v>
+      </c>
+      <c r="H30" s="4">
+        <f>H10+H26</f>
+        <v>10750.14679976512</v>
+      </c>
+      <c r="I30" s="4">
+        <f>SUM(G30:H30)</f>
+        <v>13010.863182618907</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4">
-        <f>G23+G11</f>
-        <v>720.71638285378742</v>
+        <f>G11+G27</f>
+        <v>2146.212566059894</v>
       </c>
       <c r="H31" s="4">
-        <f>H23+H11</f>
-        <v>3427.1467997651198</v>
+        <f>H11+H27</f>
+        <v>18278.03875513799</v>
       </c>
       <c r="I31" s="4">
         <f>SUM(G31:H31)</f>
-        <v>4147.8631826189076</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="4">
-        <f>G20*G12</f>
-        <v>566.39593908629433</v>
-      </c>
-      <c r="C32" s="4">
-        <f>H20*H12</f>
-        <v>5826</v>
-      </c>
+        <v>20424.251321197884</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4">
-        <f>G24+G12</f>
-        <v>684.21256605989424</v>
+        <f>SUM(G30:G31)</f>
+        <v>4406.9289489136809</v>
       </c>
       <c r="H32" s="4">
-        <f>H24+H12</f>
-        <v>5827.0387551379918</v>
-      </c>
-      <c r="I32" s="4">
-        <f>SUM(G32:H32)</f>
-        <v>6511.2513211978858</v>
-      </c>
+        <f>SUM(H30:H31)</f>
+        <v>29028.18555490311</v>
+      </c>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
@@ -5392,67 +5375,79 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4">
-        <f>SUM(G31:G32)</f>
-        <v>1404.9289489136818</v>
-      </c>
-      <c r="H33" s="4">
-        <f>SUM(H31:H32)</f>
-        <v>9254.1855549031116</v>
-      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="4">
+        <f>G22*G14</f>
+        <v>523.55772357723572</v>
+      </c>
+      <c r="C34" s="4">
+        <f>H22*H14</f>
+        <v>2648.5752961082908</v>
+      </c>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="G34" s="4">
+        <f>G26+G14</f>
+        <v>720.71638285378742</v>
+      </c>
+      <c r="H34" s="4">
+        <f>H26+H14</f>
+        <v>3427.1467997651198</v>
+      </c>
+      <c r="I34" s="4">
+        <f>SUM(G34:H34)</f>
+        <v>4147.8631826189076</v>
+      </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="B35" s="4">
+        <f>G23*G15</f>
+        <v>566.39593908629433</v>
+      </c>
+      <c r="C35" s="4">
+        <f>H23*H15</f>
+        <v>5826</v>
+      </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4">
-        <f t="shared" ref="G35:I36" si="0">G31/G27</f>
-        <v>0.31880000000000003</v>
+        <f>G27+G15</f>
+        <v>684.21256605989424</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31879999999999997</v>
+        <f>H27+H15</f>
+        <v>5827.0387551379918</v>
       </c>
       <c r="I35" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
+        <f>SUM(G35:H35)</f>
+        <v>6511.2513211978858</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
+        <f>SUM(G34:G35)</f>
+        <v>1404.9289489136818</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
-      </c>
-      <c r="I36" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
-      </c>
+        <f>SUM(H34:H35)</f>
+        <v>9254.1855549031116</v>
+      </c>
+      <c r="I36" s="4"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
@@ -5460,159 +5455,214 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4">
-        <f>G33/G29</f>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4">
+        <f t="shared" ref="G38:I39" si="0">G34/G30</f>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I38" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="I39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4">
+        <f>G36/G32</f>
         <v>0.31880000000000008</v>
       </c>
-      <c r="H37" s="4">
-        <f>H33/H29</f>
+      <c r="H40" s="4">
+        <f>H36/H32</f>
         <v>0.31880000000000003</v>
       </c>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="41" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
-      <c r="C41" s="6" t="s">
+      <c r="I40" s="4"/>
+    </row>
+    <row r="44" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C45" s="5">
         <v>750</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D45" s="5">
         <v>1238</v>
-      </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="5">
-        <v>75</v>
-      </c>
-      <c r="D43" s="5">
-        <v>498</v>
-      </c>
-      <c r="E43" s="4">
-        <f>SUM(C42:D43)</f>
-        <v>2561</v>
-      </c>
-      <c r="F43">
-        <f>D43/C43</f>
-        <v>6.64</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="4"/>
-      <c r="C44" s="4">
-        <f>C43/C42</f>
-        <v>0.1</v>
-      </c>
-      <c r="D44" s="4">
-        <f>D43/D42</f>
-        <v>0.40226171243941844</v>
-      </c>
-      <c r="E44" s="4">
-        <f>D44/C44</f>
-        <v>4.0226171243941842</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
-      <c r="C45" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E45" s="4"/>
     </row>
     <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="5">
+        <v>75</v>
+      </c>
+      <c r="D46" s="5">
+        <v>498</v>
+      </c>
+      <c r="E46" s="4">
+        <f>SUM(C45:D46)</f>
+        <v>2561</v>
+      </c>
+      <c r="F46">
+        <f>D46/C46</f>
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4">
+        <f>C46/C45</f>
+        <v>0.1</v>
+      </c>
+      <c r="D47" s="4">
+        <f>D46/D45</f>
+        <v>0.40226171243941844</v>
+      </c>
+      <c r="E47" s="4">
+        <f>D47/C47</f>
+        <v>4.0226171243941842</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C49" s="5">
         <v>267</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D49" s="5">
         <v>1721</v>
-      </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="5">
-        <v>21</v>
-      </c>
-      <c r="D47" s="5">
-        <v>552</v>
-      </c>
-      <c r="E47" s="4">
-        <f>SUM(C46:D47)</f>
-        <v>2561</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="2:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
-      <c r="C49" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="E49" s="4"/>
     </row>
     <row r="50" spans="2:5" ht="17" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="5">
+        <v>21</v>
+      </c>
+      <c r="D50" s="5">
+        <v>552</v>
+      </c>
+      <c r="E50" s="4">
+        <f>SUM(C49:D50)</f>
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C53" s="5">
         <v>881</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D53" s="5">
         <v>1107</v>
       </c>
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="2:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="B51" s="6" t="s">
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C54" s="5">
         <v>90</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D54" s="5">
         <v>483</v>
       </c>
-      <c r="E51" s="4">
-        <f>SUM(C50:D51)</f>
+      <c r="E54" s="4">
+        <f>SUM(C53:D54)</f>
         <v>2561</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{9C39114D-177D-874F-9648-8D0623AF7627}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{62BC5D29-BC2E-BE4F-9971-6E1802D9851C}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{A5515785-4094-994E-9541-747616D5BC0D}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{62FEC5B1-56D8-7740-8ED0-F73ED66D809E}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{453584B6-2853-C447-90CD-97D59EEC4005}"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{9C39114D-177D-874F-9648-8D0623AF7627}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{62BC5D29-BC2E-BE4F-9971-6E1802D9851C}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{A5515785-4094-994E-9541-747616D5BC0D}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{62FEC5B1-56D8-7740-8ED0-F73ED66D809E}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{453584B6-2853-C447-90CD-97D59EEC4005}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{EF2F4DF6-6D19-4142-A348-BD527D0C53EC}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{E8A6BA72-27D4-2445-B71B-21F775CC3AEF}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{61206B2A-15A0-EA48-9860-DCE58EE6C5D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5639,181 +5689,181 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="32" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="15"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="33" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="28">
+      <c r="E3" s="15"/>
+      <c r="F3" s="27">
         <v>5</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="27">
         <v>165</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="31" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="21" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>2.92</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>2.79</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>1.1399999999999999</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="25">
         <v>2.74</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>2.5499999999999998</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <v>4.3499999999999996</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="28">
         <v>1.19</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="28">
         <v>1.04</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="28">
         <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>0.85</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>0.85</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="22">
         <v>0.83</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="22">
         <v>0.82</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="22">
         <v>0.86</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="18"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>0.67</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="23">
         <v>0.67</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>0.65</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="23">
         <v>0.48</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="23">
         <v>0.69</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="18"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="23">
         <v>0.72</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="23">
         <v>0.75</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <v>0.64</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="23">
         <v>0.78</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="23">
         <v>0.72</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>0.62</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>0.6</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <v>0.67</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="24">
         <v>0.35</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="24">
         <v>0.66</v>
       </c>
     </row>
@@ -5834,70 +5884,70 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="12">
+      <c r="C1" s="11">
         <v>27816</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>10771</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="13"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="13"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="11"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>27816</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>3124</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>1039</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>311</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>271</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update README.md and add tests
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenamurgai/Google Drive/Projects/Insight/Project/Code/debias-ml/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6359051D-E166-724B-9001-A97F9932C574}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD54507-A701-E54C-8D4E-B18FBCCEDFA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38180" yWindow="5320" windowWidth="34960" windowHeight="23880" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
+    <workbookView xWindow="300" yWindow="1880" windowWidth="27920" windowHeight="23880" activeTab="1" xr2:uid="{49417C25-687D-6847-ABBB-850FAD07D17C}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="75">
   <si>
     <t>Training time</t>
   </si>
@@ -230,6 +230,33 @@
   </si>
   <si>
     <t>https://share.streamlit.io/0.35.0-2Ln8d/index.html?id=6emvf2pnq1BsSSNkZB6iVA</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.36.0-2Qf24/index.html?id=S5gGv8aqQyWEqdQRgXqRhA</t>
+  </si>
+  <si>
+    <t>full report</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.36.0-2Qf24/index.html?id=LJQoTeeAj5q1vjY9RgJjXG</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.36.0-2Qf24/index.html?id=ViXWqG1u1mEtwmZkWT3BkJ</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.36.0-2Qf24/index.html?id=LvNQRCRxWHEFVeUwoKBPs7</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.36.0-2Qf24/index.html?id=JDjgoPh55HrSxbKvpthCj2</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.36.0-2Qf24/index.html?id=UCo7PvitQe3DqdWrz2ZBon</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.36.0-2Qf24/index.html?id=QdPWBFJza6qoAfB1mivUm2</t>
+  </si>
+  <si>
+    <t>https://share.streamlit.io/0.36.0-2Qf24/index.html?id=R3Y8Q7cNLm56WvEb9gc9vF</t>
   </si>
 </sst>
 </file>
@@ -4808,10 +4835,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE78BA39-FCEA-B24E-B556-4309CEC91EC3}">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4821,7 +4848,7 @@
     <col min="12" max="12" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="10">
         <v>43501</v>
       </c>
@@ -4829,7 +4856,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="10">
         <v>43502</v>
       </c>
@@ -4837,7 +4864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="10">
         <v>43506</v>
       </c>
@@ -4845,7 +4872,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="10">
         <v>43507</v>
       </c>
@@ -4853,7 +4880,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="10">
         <v>43513</v>
       </c>
@@ -4861,7 +4888,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -4872,7 +4899,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -4883,7 +4910,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -4894,289 +4921,179 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="90" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1641</v>
-      </c>
-      <c r="H10" s="5">
-        <v>8305</v>
-      </c>
-      <c r="I10" s="4">
-        <f>SUM(G10:H10)</f>
-        <v>9946</v>
-      </c>
-      <c r="N10">
-        <f>N11/(N11+N12)</f>
-        <v>0.88618285679186759</v>
-      </c>
-      <c r="O10">
-        <f>M13/SUM(M13:M18)</f>
-        <v>0.8542735173981143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <f>SUM(G10:H11)</f>
-        <v>30000</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1777</v>
-      </c>
-      <c r="H11" s="5">
-        <v>18277</v>
-      </c>
-      <c r="I11" s="4">
-        <f>SUM(G11:H11)</f>
-        <v>20054</v>
-      </c>
-      <c r="N11">
-        <f>M13+M15</f>
-        <v>28855</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4">
-        <f>SUM(G10:G11)</f>
-        <v>3418</v>
-      </c>
-      <c r="H12" s="4">
-        <f>SUM(H10:H11)</f>
-        <v>26582</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="N12">
-        <f>M14+M16+M17</f>
-        <v>3706</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="L13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" s="9">
-        <v>27816</v>
-      </c>
-      <c r="N13" s="7">
-        <f>M13/SUM($M$13:$M$17)</f>
-        <v>0.8542735173981143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="5">
-        <v>101</v>
-      </c>
-      <c r="H14" s="5">
-        <v>982</v>
-      </c>
-      <c r="I14" s="4">
-        <f>SUM(G14:H14)</f>
-        <v>1083</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="9">
-        <v>3124</v>
-      </c>
-      <c r="N14" s="7">
-        <f>M14/SUM($M$13:$M$17)</f>
-        <v>9.5942999293633494E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="5">
-        <v>315</v>
-      </c>
-      <c r="H15" s="5">
-        <v>5826</v>
-      </c>
-      <c r="I15" s="4">
-        <f>SUM(G15:H15)</f>
-        <v>6141</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="9">
-        <v>1039</v>
-      </c>
-      <c r="N15" s="7">
-        <f>M15/SUM($M$13:$M$17)</f>
-        <v>3.1909339393753261E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4">
-        <f>SUM(G14:G15)</f>
-        <v>416</v>
-      </c>
-      <c r="H16" s="4">
-        <f>SUM(H14:H15)</f>
-        <v>6808</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="L16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="M16" s="9">
-        <v>311</v>
-      </c>
-      <c r="N16" s="7">
-        <f>M16/SUM($M$13:$M$17)</f>
-        <v>9.551303706888609E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="10">
+        <v>43588</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="10">
+        <v>43588</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="10">
+        <v>43588</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="10">
+        <v>43588</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="10">
+        <v>43590</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="10">
+        <v>43590</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="10">
+        <v>43590</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="10">
+        <v>43590</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="L17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" s="9">
-        <v>271</v>
-      </c>
-      <c r="N17" s="7">
-        <f>M17/SUM($M$13:$M$17)</f>
-        <v>8.3228402076103315E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" ht="17" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
-        <f>G14/G10</f>
-        <v>6.1547836684948204E-2</v>
-      </c>
-      <c r="C18" s="4">
-        <f>H14/H10</f>
-        <v>0.11824202287778447</v>
-      </c>
-      <c r="D18" s="4"/>
+      <c r="G17" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="17" x14ac:dyDescent="0.25">
       <c r="E18" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="5">
-        <v>6.1499999999999999E-2</v>
+        <v>1641</v>
       </c>
       <c r="H18" s="5">
-        <v>0.1182</v>
+        <v>8305</v>
       </c>
       <c r="I18" s="4">
-        <f>I14/I10</f>
-        <v>0.10888799517393927</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" ht="17" x14ac:dyDescent="0.25">
+        <f>SUM(G18:H18)</f>
+        <v>9946</v>
+      </c>
+      <c r="N18">
+        <f>N19/(N19+N20)</f>
+        <v>0.88618285679186759</v>
+      </c>
+      <c r="O18">
+        <f>M21/SUM(M21:M26)</f>
+        <v>0.8542735173981143</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
-        <f>G15/G11</f>
-        <v>0.17726505346088914</v>
-      </c>
-      <c r="C19" s="4">
-        <f>H15/H11</f>
-        <v>0.31876128467472781</v>
-      </c>
+        <f>SUM(G18:H19)</f>
+        <v>30000</v>
+      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E19" s="4"/>
       <c r="F19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G19" s="5">
-        <v>0.17730000000000001</v>
+        <v>1777</v>
       </c>
       <c r="H19" s="5">
-        <v>0.31879999999999997</v>
+        <v>18277</v>
       </c>
       <c r="I19" s="4">
-        <f>I15/I11</f>
-        <v>0.30622319736710879</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+        <f>SUM(G19:H19)</f>
+        <v>20054</v>
+      </c>
+      <c r="N19">
+        <f>M21+M23</f>
+        <v>28855</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4">
-        <f>G16/G12</f>
-        <v>0.12170860152135751</v>
+        <f>SUM(G18:G19)</f>
+        <v>3418</v>
       </c>
       <c r="H20" s="4">
-        <f>H16/H12</f>
-        <v>0.25611315928071626</v>
+        <f>SUM(H18:H19)</f>
+        <v>26582</v>
       </c>
       <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N20">
+        <f>M22+M24+M25</f>
+        <v>3706</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -5185,125 +5102,196 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="9">
+        <v>27816</v>
+      </c>
+      <c r="N21" s="7">
+        <f>M21/SUM($M$21:$M$25)</f>
+        <v>0.8542735173981143</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4">
-        <f>$H$19/G18</f>
-        <v>5.1837398373983739</v>
-      </c>
-      <c r="H22" s="4">
-        <f>$H$19/H18</f>
-        <v>2.6971235194585446</v>
+        <v>28</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="5">
+        <v>101</v>
+      </c>
+      <c r="H22" s="5">
+        <v>982</v>
       </c>
       <c r="I22" s="4">
-        <f>I19/I18</f>
-        <v>2.8122769353769752</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+        <f>SUM(G22:H22)</f>
+        <v>1083</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="9">
+        <v>3124</v>
+      </c>
+      <c r="N22" s="7">
+        <f>M22/SUM($M$21:$M$25)</f>
+        <v>9.5942999293633494E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4">
-        <f>$H$19/G19</f>
-        <v>1.7980823463056963</v>
-      </c>
-      <c r="H23" s="4">
-        <f>$H$19/H19</f>
-        <v>1</v>
-      </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B24">
-        <v>619.58789999999999</v>
-      </c>
-      <c r="C24">
-        <v>2444.5385999999999</v>
-      </c>
+      <c r="E23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="5">
+        <v>315</v>
+      </c>
+      <c r="H23" s="5">
+        <v>5826</v>
+      </c>
+      <c r="I23" s="4">
+        <f>SUM(G23:H23)</f>
+        <v>6141</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="9">
+        <v>1039</v>
+      </c>
+      <c r="N23" s="7">
+        <f>M23/SUM($M$21:$M$25)</f>
+        <v>3.1909339393753261E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4">
+        <f>SUM(G22:G23)</f>
+        <v>416</v>
+      </c>
       <c r="H24" s="4">
-        <f>H20/G20</f>
-        <v>2.1043143712055006</v>
+        <f>SUM(H22:H23)</f>
+        <v>6808</v>
       </c>
       <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <v>369.09059999999999</v>
-      </c>
+      <c r="L24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="9">
+        <v>311</v>
+      </c>
+      <c r="N24" s="7">
+        <f>M24/SUM($M$21:$M$25)</f>
+        <v>9.551303706888609E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="9">
+        <v>271</v>
+      </c>
+      <c r="N25" s="7">
+        <f>M25/SUM($M$21:$M$25)</f>
+        <v>8.3228402076103315E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
-        <v>422.55772357723578</v>
+        <f>G22/G18</f>
+        <v>6.1547836684948204E-2</v>
       </c>
       <c r="C26" s="4">
-        <v>1666.5752961082908</v>
+        <f>H22/H18</f>
+        <v>0.11824202287778447</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4">
-        <f>($H$19*G10 - G14)/(1 - $H$19)</f>
-        <v>619.71638285378742</v>
-      </c>
-      <c r="H26" s="4">
-        <f>($H$19*H10-H14)/(1-$H$19)</f>
-        <v>2445.1467997651198</v>
-      </c>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="5">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.1182</v>
+      </c>
+      <c r="I26" s="4">
+        <f>I22/I18</f>
+        <v>0.10888799517393927</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="17" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
-        <v>251.39593908629433</v>
+        <f>G23/G19</f>
+        <v>0.17726505346088914</v>
       </c>
       <c r="C27" s="4">
-        <v>0</v>
+        <f>H23/H19</f>
+        <v>0.31876128467472781</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4">
-        <f>($H$19*G11-G15)/(1-$H$19)</f>
-        <v>369.21256605989419</v>
-      </c>
-      <c r="H27" s="4">
-        <f>($H$19*H11-H15)/(1-$H$19)</f>
-        <v>1.0387551379913817</v>
-      </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.17730000000000001</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I27" s="4">
+        <f>I23/I19</f>
+        <v>0.30622319736710879</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="G28" s="4">
+        <f>G24/G20</f>
+        <v>0.12170860152135751</v>
+      </c>
+      <c r="H28" s="4">
+        <f>H24/H20</f>
+        <v>0.25611315928071626</v>
+      </c>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -5313,65 +5301,64 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4">
-        <f>G10+G26</f>
-        <v>2260.7163828537873</v>
+        <f>$H$27/G26</f>
+        <v>5.1837398373983739</v>
       </c>
       <c r="H30" s="4">
-        <f>H10+H26</f>
-        <v>10750.14679976512</v>
+        <f>$H$27/H26</f>
+        <v>2.6971235194585446</v>
       </c>
       <c r="I30" s="4">
-        <f>SUM(G30:H30)</f>
-        <v>13010.863182618907</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+        <f>I27/I26</f>
+        <v>2.8122769353769752</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4">
-        <f>G11+G27</f>
-        <v>2146.212566059894</v>
+        <f>$H$27/G27</f>
+        <v>1.7980823463056963</v>
       </c>
       <c r="H31" s="4">
-        <f>H11+H27</f>
-        <v>18278.03875513799</v>
-      </c>
-      <c r="I31" s="4">
-        <f>SUM(G31:H31)</f>
-        <v>20424.251321197884</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+        <f>$H$27/H27</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>619.58789999999999</v>
+      </c>
+      <c r="C32">
+        <v>2444.5385999999999</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4">
-        <f>SUM(G30:G31)</f>
-        <v>4406.9289489136809</v>
-      </c>
+      <c r="G32" s="4"/>
       <c r="H32" s="4">
-        <f>SUM(H30:H31)</f>
-        <v>29028.18555490311</v>
+        <f>H28/G28</f>
+        <v>2.1043143712055006</v>
       </c>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="B33">
+        <v>369.09059999999999</v>
+      </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -5381,57 +5368,45 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="4">
-        <f>G22*G14</f>
-        <v>523.55772357723572</v>
+        <v>422.55772357723578</v>
       </c>
       <c r="C34" s="4">
-        <f>H22*H14</f>
-        <v>2648.5752961082908</v>
+        <v>1666.5752961082908</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4">
-        <f>G26+G14</f>
-        <v>720.71638285378742</v>
+        <f>($H$27*G18 - G22)/(1 - $H$27)</f>
+        <v>619.71638285378742</v>
       </c>
       <c r="H34" s="4">
-        <f>H26+H14</f>
-        <v>3427.1467997651198</v>
-      </c>
-      <c r="I34" s="4">
-        <f>SUM(G34:H34)</f>
-        <v>4147.8631826189076</v>
-      </c>
+        <f>($H$27*H18-H22)/(1-$H$27)</f>
+        <v>2445.1467997651198</v>
+      </c>
+      <c r="I34" s="4"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="4">
-        <f>G23*G15</f>
-        <v>566.39593908629433</v>
+        <v>251.39593908629433</v>
       </c>
       <c r="C35" s="4">
-        <f>H23*H15</f>
-        <v>5826</v>
+        <v>0</v>
       </c>
       <c r="D35" s="4"/>
-      <c r="E35" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4">
-        <f>G27+G15</f>
-        <v>684.21256605989424</v>
+        <f>($H$27*G19-G23)/(1-$H$27)</f>
+        <v>369.21256605989419</v>
       </c>
       <c r="H35" s="4">
-        <f>H27+H15</f>
-        <v>5827.0387551379918</v>
-      </c>
-      <c r="I35" s="4">
-        <f>SUM(G35:H35)</f>
-        <v>6511.2513211978858</v>
-      </c>
+        <f>($H$27*H19-H23)/(1-$H$27)</f>
+        <v>1.0387551379913817</v>
+      </c>
+      <c r="I35" s="4"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
@@ -5439,14 +5414,8 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="4">
-        <f>SUM(G34:G35)</f>
-        <v>1404.9289489136818</v>
-      </c>
-      <c r="H36" s="4">
-        <f>SUM(H34:H35)</f>
-        <v>9254.1855549031116</v>
-      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
@@ -5464,41 +5433,39 @@
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4">
-        <f t="shared" ref="G38:I39" si="0">G34/G30</f>
-        <v>0.31880000000000003</v>
+        <f>G18+G34</f>
+        <v>2260.7163828537873</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31879999999999997</v>
+        <f>H18+H34</f>
+        <v>10750.14679976512</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
+        <f>SUM(G38:H38)</f>
+        <v>13010.863182618907</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
+        <f>G19+G35</f>
+        <v>2146.212566059894</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
+        <f>H19+H35</f>
+        <v>18278.03875513799</v>
       </c>
       <c r="I39" s="4">
-        <f t="shared" si="0"/>
-        <v>0.31880000000000003</v>
+        <f>SUM(G39:H39)</f>
+        <v>20424.251321197884</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
@@ -5508,148 +5475,296 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4">
-        <f>G36/G32</f>
-        <v>0.31880000000000008</v>
+        <f>SUM(G38:G39)</f>
+        <v>4406.9289489136809</v>
       </c>
       <c r="H40" s="4">
-        <f>H36/H32</f>
+        <f>SUM(H38:H39)</f>
+        <v>29028.18555490311</v>
+      </c>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="4">
+        <f>G30*G22</f>
+        <v>523.55772357723572</v>
+      </c>
+      <c r="C42" s="4">
+        <f>H30*H22</f>
+        <v>2648.5752961082908</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4">
+        <f>G34+G22</f>
+        <v>720.71638285378742</v>
+      </c>
+      <c r="H42" s="4">
+        <f>H34+H22</f>
+        <v>3427.1467997651198</v>
+      </c>
+      <c r="I42" s="4">
+        <f>SUM(G42:H42)</f>
+        <v>4147.8631826189076</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="4">
+        <f>G31*G23</f>
+        <v>566.39593908629433</v>
+      </c>
+      <c r="C43" s="4">
+        <f>H31*H23</f>
+        <v>5826</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4">
+        <f>G35+G23</f>
+        <v>684.21256605989424</v>
+      </c>
+      <c r="H43" s="4">
+        <f>H35+H23</f>
+        <v>5827.0387551379918</v>
+      </c>
+      <c r="I43" s="4">
+        <f>SUM(G43:H43)</f>
+        <v>6511.2513211978858</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4">
+        <f>SUM(G42:G43)</f>
+        <v>1404.9289489136818</v>
+      </c>
+      <c r="H44" s="4">
+        <f>SUM(H42:H43)</f>
+        <v>9254.1855549031116</v>
+      </c>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4">
+        <f t="shared" ref="G46:I47" si="0">G42/G38</f>
         <v>0.31880000000000003</v>
       </c>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="44" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
-      <c r="C44" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="5">
-        <v>750</v>
-      </c>
-      <c r="D45" s="5">
-        <v>1238</v>
-      </c>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="5">
-        <v>75</v>
-      </c>
-      <c r="D46" s="5">
-        <v>498</v>
-      </c>
-      <c r="E46" s="4">
-        <f>SUM(C45:D46)</f>
-        <v>2561</v>
-      </c>
-      <c r="F46">
-        <f>D46/C46</f>
-        <v>6.64</v>
+      <c r="H46" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31879999999999997</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="4">
-        <f>C46/C45</f>
-        <v>0.1</v>
-      </c>
-      <c r="D47" s="4">
-        <f>D46/D45</f>
-        <v>0.40226171243941844</v>
-      </c>
-      <c r="E47" s="4">
-        <f>D47/C47</f>
-        <v>4.0226171243941842</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" ht="17" x14ac:dyDescent="0.25">
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="H47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="I47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31880000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
-      <c r="C48" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
       <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="2:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="B49" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" s="5">
-        <v>267</v>
-      </c>
-      <c r="D49" s="5">
-        <v>1721</v>
-      </c>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="2:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="B50" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" s="5">
-        <v>21</v>
-      </c>
-      <c r="D50" s="5">
-        <v>552</v>
-      </c>
-      <c r="E50" s="4">
-        <f>SUM(C49:D50)</f>
-        <v>2561</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="F48" s="4"/>
+      <c r="G48" s="4">
+        <f>G44/G40</f>
+        <v>0.31880000000000008</v>
+      </c>
+      <c r="H48" s="4">
+        <f>H44/H40</f>
+        <v>0.31880000000000003</v>
+      </c>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="52" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E52" s="4"/>
     </row>
-    <row r="53" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="5">
-        <v>881</v>
+        <v>750</v>
       </c>
       <c r="D53" s="5">
-        <v>1107</v>
+        <v>1238</v>
       </c>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="2:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C54" s="5">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="D54" s="5">
-        <v>483</v>
+        <v>498</v>
       </c>
       <c r="E54" s="4">
         <f>SUM(C53:D54)</f>
+        <v>2561</v>
+      </c>
+      <c r="F54">
+        <f>D54/C54</f>
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4">
+        <f>C54/C53</f>
+        <v>0.1</v>
+      </c>
+      <c r="D55" s="4">
+        <f>D54/D53</f>
+        <v>0.40226171243941844</v>
+      </c>
+      <c r="E55" s="4">
+        <f>D55/C55</f>
+        <v>4.0226171243941842</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="5">
+        <v>267</v>
+      </c>
+      <c r="D57" s="5">
+        <v>1721</v>
+      </c>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" s="5">
+        <v>21</v>
+      </c>
+      <c r="D58" s="5">
+        <v>552</v>
+      </c>
+      <c r="E58" s="4">
+        <f>SUM(C57:D58)</f>
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="C60" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="5">
+        <v>881</v>
+      </c>
+      <c r="D61" s="5">
+        <v>1107</v>
+      </c>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="5">
+        <v>90</v>
+      </c>
+      <c r="D62" s="5">
+        <v>483</v>
+      </c>
+      <c r="E62" s="4">
+        <f>SUM(C61:D62)</f>
         <v>2561</v>
       </c>
     </row>
@@ -5663,6 +5778,14 @@
     <hyperlink ref="C6" r:id="rId6" xr:uid="{EF2F4DF6-6D19-4142-A348-BD527D0C53EC}"/>
     <hyperlink ref="C7" r:id="rId7" xr:uid="{E8A6BA72-27D4-2445-B71B-21F775CC3AEF}"/>
     <hyperlink ref="C8" r:id="rId8" xr:uid="{61206B2A-15A0-EA48-9860-DCE58EE6C5D4}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{2F29161E-1E7E-8D40-9957-3DDC138020E2}"/>
+    <hyperlink ref="C10" r:id="rId10" xr:uid="{5D849A9F-EFAA-D743-BD2A-5A9A13EBD284}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{D047529A-14F3-2045-A8C7-9BAED7C2D632}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{F63CE030-27B9-7840-8547-772F57B7A569}"/>
+    <hyperlink ref="C13" r:id="rId13" xr:uid="{A6EE4ABD-194C-6F4F-BA79-4BB4B0F1E6BB}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{71EEFF03-7CC2-F24E-9DBF-8CD114C906A5}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{0CA7EA27-5E66-8E4B-A676-6EC47AB78F34}"/>
+    <hyperlink ref="C16" r:id="rId16" xr:uid="{A81C4DA9-8D78-094D-8258-88FC0A9D3FB9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>